<commit_message>
finished: get valid extension. Next is get unique extension from d_validExtension
</commit_message>
<xml_diff>
--- a/MyThesis.xlsx
+++ b/MyThesis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6870" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6870" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="278">
   <si>
     <t>A</t>
   </si>
@@ -967,18 +967,9 @@
     <t>d*=2</t>
   </si>
   <si>
-    <t>EXT</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
-    <t>scan V</t>
-  </si>
-  <si>
-    <t>Vext</t>
-  </si>
-  <si>
     <t>idx</t>
   </si>
   <si>
@@ -1000,9 +991,6 @@
     <t>Extract the valid extensions</t>
   </si>
   <si>
-    <t>Vunique</t>
-  </si>
-  <si>
     <t>Extract the unique extensions</t>
   </si>
   <si>
@@ -1040,13 +1028,25 @@
   </si>
   <si>
     <t>Dựa vào đâu để biết DFS Code của edge extension?</t>
+  </si>
+  <si>
+    <t>d_ValidExtension</t>
+  </si>
+  <si>
+    <t>d_UniqueExtension</t>
+  </si>
+  <si>
+    <t>d_Extension</t>
+  </si>
+  <si>
+    <t>scan V: index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1149,6 +1149,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1814,7 +1821,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2134,6 +2141,18 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2164,6 +2183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6432,36 +6452,36 @@
       <c r="B35" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="167" t="s">
+      <c r="C35" s="171" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="162"/>
-      <c r="E35" s="163"/>
-      <c r="F35" s="167" t="s">
+      <c r="D35" s="166"/>
+      <c r="E35" s="167"/>
+      <c r="F35" s="171" t="s">
         <v>74</v>
       </c>
-      <c r="G35" s="162"/>
-      <c r="H35" s="163"/>
-      <c r="I35" s="167" t="s">
+      <c r="G35" s="166"/>
+      <c r="H35" s="167"/>
+      <c r="I35" s="171" t="s">
         <v>80</v>
       </c>
-      <c r="J35" s="162"/>
-      <c r="K35" s="163"/>
-      <c r="L35" s="167" t="s">
+      <c r="J35" s="166"/>
+      <c r="K35" s="167"/>
+      <c r="L35" s="171" t="s">
         <v>82</v>
       </c>
-      <c r="M35" s="162"/>
-      <c r="N35" s="163"/>
-      <c r="O35" s="167" t="s">
+      <c r="M35" s="166"/>
+      <c r="N35" s="167"/>
+      <c r="O35" s="171" t="s">
         <v>84</v>
       </c>
-      <c r="P35" s="162"/>
-      <c r="Q35" s="163"/>
-      <c r="R35" s="161" t="s">
+      <c r="P35" s="166"/>
+      <c r="Q35" s="167"/>
+      <c r="R35" s="165" t="s">
         <v>91</v>
       </c>
-      <c r="S35" s="162"/>
-      <c r="T35" s="163"/>
+      <c r="S35" s="166"/>
+      <c r="T35" s="167"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B36" s="50" t="s">
@@ -6604,16 +6624,16 @@
       <c r="B48" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="164" t="s">
+      <c r="C48" s="168" t="s">
         <v>70</v>
       </c>
-      <c r="D48" s="165"/>
-      <c r="E48" s="166"/>
-      <c r="F48" s="167" t="s">
+      <c r="D48" s="169"/>
+      <c r="E48" s="170"/>
+      <c r="F48" s="171" t="s">
         <v>74</v>
       </c>
-      <c r="G48" s="162"/>
-      <c r="H48" s="163"/>
+      <c r="G48" s="166"/>
+      <c r="H48" s="167"/>
     </row>
     <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" s="33" t="s">
@@ -6978,14 +6998,14 @@
     </row>
     <row r="58" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="159" t="s">
+      <c r="C59" s="163" t="s">
         <v>102</v>
       </c>
-      <c r="D59" s="160"/>
-      <c r="F59" s="159" t="s">
+      <c r="D59" s="164"/>
+      <c r="F59" s="163" t="s">
         <v>103</v>
       </c>
-      <c r="G59" s="160"/>
+      <c r="G59" s="164"/>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B60">
@@ -12137,13 +12157,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="AL15" sqref="AL15:AO15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="159" bestFit="1" customWidth="1"/>
     <col min="2" max="33" width="4.7109375" customWidth="1"/>
     <col min="34" max="34" width="5.5703125" customWidth="1"/>
     <col min="35" max="42" width="4.85546875" customWidth="1"/>
@@ -12151,111 +12171,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>253</v>
+      <c r="B1" s="144" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
+      <c r="A2" s="160" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="161">
+        <v>0</v>
+      </c>
+      <c r="C2" s="161">
+        <v>1</v>
+      </c>
+      <c r="D2" s="161">
+        <v>2</v>
+      </c>
+      <c r="E2" s="161">
+        <v>3</v>
+      </c>
+      <c r="F2" s="161">
+        <v>4</v>
+      </c>
+      <c r="G2" s="161">
         <v>5</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="161">
         <v>6</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="161">
         <v>7</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="161">
         <v>8</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="161">
         <v>9</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="161">
         <v>10</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="161">
         <v>11</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="161">
         <v>12</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="161">
         <v>13</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="161">
         <v>14</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="161">
         <v>15</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="161">
         <v>16</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="161">
         <v>17</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="161">
         <v>18</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="161">
         <v>19</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="161">
         <v>20</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="161">
         <v>21</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="161">
         <v>22</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="161">
         <v>23</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="161">
         <v>24</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="161">
         <v>25</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="161">
         <v>26</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="161">
         <v>27</v>
       </c>
-      <c r="AD2">
+      <c r="AD2" s="161">
         <v>28</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" s="161">
         <v>29</v>
       </c>
-      <c r="AF2">
+      <c r="AF2" s="161">
         <v>30</v>
       </c>
-      <c r="AG2">
+      <c r="AG2" s="161">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:34" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="148" t="s">
-        <v>258</v>
+      <c r="A3" s="154" t="s">
+        <v>255</v>
       </c>
       <c r="B3" s="26">
         <v>0</v>
@@ -12355,8 +12378,8 @@
       </c>
     </row>
     <row r="4" spans="1:34" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="148" t="s">
-        <v>259</v>
+      <c r="A4" s="154" t="s">
+        <v>256</v>
       </c>
       <c r="B4" s="26">
         <v>1</v>
@@ -12456,8 +12479,8 @@
       </c>
     </row>
     <row r="5" spans="1:34" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="148" t="s">
-        <v>260</v>
+      <c r="A5" s="154" t="s">
+        <v>257</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>0</v>
@@ -12557,8 +12580,8 @@
       </c>
     </row>
     <row r="6" spans="1:34" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="148" t="s">
-        <v>261</v>
+      <c r="A6" s="154" t="s">
+        <v>258</v>
       </c>
       <c r="B6" s="26" t="s">
         <v>1</v>
@@ -12657,12 +12680,12 @@
         <v>4</v>
       </c>
       <c r="AH6" s="150" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:34" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="148" t="s">
-        <v>254</v>
+      <c r="A7" s="154" t="s">
+        <v>253</v>
       </c>
       <c r="B7" s="148">
         <f>IF(B5&lt;=B6,1,0)</f>
@@ -12798,201 +12821,201 @@
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>255</v>
+      <c r="A8" s="159" t="s">
+        <v>277</v>
       </c>
       <c r="B8" s="149">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="162">
         <f>B8+B7</f>
         <v>1</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="162">
         <f t="shared" ref="D8:AG8" si="1">C8+C7</f>
         <v>2</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="162">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="162">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="162">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="162">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="162">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="162">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="162">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="162">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="162">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="162">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="162">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="162">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="162">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="162">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="162">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="162">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="162">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="162">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="W8">
+      <c r="W8" s="162">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="X8">
+      <c r="X8" s="162">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="Y8">
+      <c r="Y8" s="162">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="Z8">
+      <c r="Z8" s="162">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="AA8">
+      <c r="AA8" s="162">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="AB8">
+      <c r="AB8" s="162">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="AC8">
+      <c r="AC8" s="162">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="AD8">
+      <c r="AD8" s="162">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="AE8">
+      <c r="AE8" s="162">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="AF8">
+      <c r="AF8" s="162">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="AG8">
+      <c r="AG8" s="162">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>257</v>
+      <c r="A9" s="159" t="s">
+        <v>112</v>
       </c>
       <c r="B9" s="149">
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="162">
         <v>1</v>
       </c>
       <c r="D9" s="149">
         <v>2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="162">
         <v>3</v>
       </c>
       <c r="F9" s="149">
         <v>4</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="162">
         <v>5</v>
       </c>
       <c r="H9" s="149">
         <v>6</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="162">
         <v>7</v>
       </c>
       <c r="J9" s="149">
         <v>8</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="162">
         <v>9</v>
       </c>
       <c r="L9" s="149">
         <v>10</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="162">
         <v>11</v>
       </c>
       <c r="N9" s="149">
         <v>12</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="162">
         <v>13</v>
       </c>
       <c r="P9" s="149">
         <v>14</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="162">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="144" t="s">
-        <v>256</v>
+      <c r="A10" s="153" t="s">
+        <v>274</v>
       </c>
       <c r="B10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" s="148" t="s">
-        <v>258</v>
+      <c r="A11" s="154" t="s">
+        <v>255</v>
       </c>
       <c r="B11" s="26">
         <v>0</v>
@@ -13044,8 +13067,8 @@
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" s="148" t="s">
-        <v>259</v>
+      <c r="A12" s="154" t="s">
+        <v>256</v>
       </c>
       <c r="B12" s="26">
         <v>1</v>
@@ -13097,8 +13120,8 @@
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="148" t="s">
-        <v>260</v>
+      <c r="A13" s="154" t="s">
+        <v>257</v>
       </c>
       <c r="B13" s="26" t="s">
         <v>0</v>
@@ -13150,122 +13173,122 @@
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="148" t="s">
+      <c r="A14" s="154" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="M14" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="N14" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="O14" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A15" s="154" t="s">
+        <v>253</v>
+      </c>
+      <c r="B15" s="148">
+        <v>1</v>
+      </c>
+      <c r="C15" s="148">
+        <v>1</v>
+      </c>
+      <c r="D15" s="148">
+        <v>1</v>
+      </c>
+      <c r="E15" s="148">
+        <v>1</v>
+      </c>
+      <c r="F15" s="148">
+        <v>1</v>
+      </c>
+      <c r="G15" s="148">
+        <v>1</v>
+      </c>
+      <c r="H15" s="148">
+        <v>1</v>
+      </c>
+      <c r="I15" s="148">
+        <v>1</v>
+      </c>
+      <c r="J15" s="148">
+        <v>1</v>
+      </c>
+      <c r="K15" s="148">
+        <v>1</v>
+      </c>
+      <c r="L15" s="148">
+        <v>1</v>
+      </c>
+      <c r="M15" s="148">
+        <v>1</v>
+      </c>
+      <c r="N15" s="148">
+        <v>1</v>
+      </c>
+      <c r="O15" s="148">
+        <v>1</v>
+      </c>
+      <c r="P15" s="148">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16" s="157" t="s">
+        <v>275</v>
+      </c>
+      <c r="B16" t="s">
         <v>261</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="L14" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="M14" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="N14" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="O14" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="P14" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" s="148" t="s">
-        <v>254</v>
-      </c>
-      <c r="B15" s="148">
-        <v>1</v>
-      </c>
-      <c r="C15" s="148">
-        <v>1</v>
-      </c>
-      <c r="D15" s="148">
-        <v>1</v>
-      </c>
-      <c r="E15" s="148">
-        <v>1</v>
-      </c>
-      <c r="F15" s="148">
-        <v>1</v>
-      </c>
-      <c r="G15" s="148">
-        <v>1</v>
-      </c>
-      <c r="H15" s="148">
-        <v>1</v>
-      </c>
-      <c r="I15" s="148">
-        <v>1</v>
-      </c>
-      <c r="J15" s="148">
-        <v>1</v>
-      </c>
-      <c r="K15" s="148">
-        <v>1</v>
-      </c>
-      <c r="L15" s="148">
-        <v>1</v>
-      </c>
-      <c r="M15" s="148">
-        <v>1</v>
-      </c>
-      <c r="N15" s="148">
-        <v>1</v>
-      </c>
-      <c r="O15" s="148">
-        <v>1</v>
-      </c>
-      <c r="P15" s="148">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="148">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" s="151" t="s">
-        <v>264</v>
-      </c>
-      <c r="B16" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B17" s="152" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F17">
         <v>5</v>
@@ -13277,89 +13300,89 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B18" s="152" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19" s="153" t="s">
-        <v>257</v>
-      </c>
-      <c r="B19" s="144">
-        <v>0</v>
-      </c>
-      <c r="C19" s="144">
-        <v>1</v>
-      </c>
-      <c r="D19" s="144">
-        <v>2</v>
-      </c>
-      <c r="E19" s="144">
-        <v>3</v>
-      </c>
-      <c r="F19" s="144">
-        <v>4</v>
-      </c>
-      <c r="G19" s="144">
+      <c r="A19" s="160" t="s">
+        <v>254</v>
+      </c>
+      <c r="B19" s="173">
+        <v>0</v>
+      </c>
+      <c r="C19" s="173">
+        <v>1</v>
+      </c>
+      <c r="D19" s="173">
+        <v>2</v>
+      </c>
+      <c r="E19" s="173">
+        <v>3</v>
+      </c>
+      <c r="F19" s="173">
+        <v>4</v>
+      </c>
+      <c r="G19" s="173">
         <v>5</v>
       </c>
-      <c r="H19" s="144">
+      <c r="H19" s="173">
         <v>6</v>
       </c>
-      <c r="I19" s="144">
+      <c r="I19" s="173">
         <v>7</v>
       </c>
-      <c r="J19" s="144">
+      <c r="J19" s="173">
         <v>8</v>
       </c>
-      <c r="K19" s="144">
+      <c r="K19" s="173">
         <v>9</v>
       </c>
-      <c r="L19" s="144">
+      <c r="L19" s="173">
         <v>10</v>
       </c>
-      <c r="M19" s="144">
+      <c r="M19" s="173">
         <v>11</v>
       </c>
-      <c r="N19" s="144">
+      <c r="N19" s="173">
         <v>12</v>
       </c>
-      <c r="O19" s="144">
+      <c r="O19" s="173">
         <v>13</v>
       </c>
-      <c r="P19" s="144">
+      <c r="P19" s="173">
         <v>14</v>
       </c>
-      <c r="Q19" s="144">
+      <c r="Q19" s="173">
         <v>15</v>
       </c>
-      <c r="R19" s="144">
+      <c r="R19" s="173">
         <v>16</v>
       </c>
-      <c r="S19" s="144">
+      <c r="S19" s="173">
         <v>17</v>
       </c>
-      <c r="T19" s="144">
+      <c r="T19" s="173">
         <v>18</v>
       </c>
-      <c r="U19" s="144">
+      <c r="U19" s="173">
         <v>19</v>
       </c>
-      <c r="V19" s="144">
+      <c r="V19" s="173">
         <v>20</v>
       </c>
-      <c r="W19" s="144">
+      <c r="W19" s="173">
         <v>21</v>
       </c>
-      <c r="X19" s="144">
+      <c r="X19" s="173">
         <v>22</v>
       </c>
-      <c r="Y19" s="144">
+      <c r="Y19" s="173">
         <v>23</v>
       </c>
-      <c r="Z19" s="144">
+      <c r="Z19" s="173">
         <v>24</v>
       </c>
     </row>
@@ -13521,7 +13544,7 @@
     </row>
     <row r="22" spans="1:27" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="154" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B22" s="26">
         <v>0</v>
@@ -13601,7 +13624,7 @@
     </row>
     <row r="23" spans="1:27" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="154" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B23" s="26">
         <v>0</v>
@@ -13681,7 +13704,7 @@
     </row>
     <row r="24" spans="1:27" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="154" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B24" s="26">
         <v>0</v>
@@ -13761,7 +13784,7 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="155" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B25" s="144">
         <f>B22*$F$17*$F$18+B24*$F$17+B23</f>
@@ -13864,12 +13887,12 @@
         <v>24</v>
       </c>
       <c r="AA25" s="158" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:27" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="154" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B26" s="26">
         <v>0</v>
@@ -13953,7 +13976,7 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="156" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B27" s="149">
         <v>0</v>
@@ -14057,7 +14080,7 @@
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="157" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B28" s="151">
         <v>0</v>
@@ -14083,7 +14106,7 @@
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="156" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B29" s="148" t="s">
         <v>0</v>
@@ -14133,7 +14156,7 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="154" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B31" s="26">
         <v>0</v>
@@ -14159,7 +14182,7 @@
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="154" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B32" s="26">
         <v>1</v>
@@ -14185,7 +14208,7 @@
     </row>
     <row r="33" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A33" s="154" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B33" s="26">
         <v>0</v>
@@ -14211,7 +14234,7 @@
     </row>
     <row r="34" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A34" s="154" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B34" s="26">
         <v>1</v>
@@ -14238,12 +14261,12 @@
     <row r="35" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A35" s="156"/>
       <c r="B35" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="36" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B36" s="152" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F36">
         <v>5</v>
@@ -14251,7 +14274,7 @@
     </row>
     <row r="37" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B37" s="152" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F37">
         <v>2</v>
@@ -14259,7 +14282,7 @@
     </row>
     <row r="39" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B39" s="153" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C39" s="144">
         <v>0</v>
@@ -14645,7 +14668,7 @@
     </row>
     <row r="42" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B42" s="154" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C42" s="26">
         <v>0</v>
@@ -14800,7 +14823,7 @@
     </row>
     <row r="43" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B43" s="154" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C43" s="26">
         <v>0</v>
@@ -14955,7 +14978,7 @@
     </row>
     <row r="44" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B44" s="154" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C44" s="26">
         <v>0</v>
@@ -15110,7 +15133,7 @@
     </row>
     <row r="45" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B45" s="155" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C45" s="144">
         <f>C42*$F$36*$F$37+C44*$F$36+C43</f>
@@ -15315,7 +15338,7 @@
     </row>
     <row r="47" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B47" s="156" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C47">
         <f t="shared" ref="C47:AZ47" si="5">INT(C45/(5*2))</f>
@@ -15520,7 +15543,7 @@
     </row>
     <row r="48" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B48" s="156" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C48">
         <f t="shared" ref="C48:AZ48" si="6">MOD(C45,5*2)</f>
@@ -15724,10 +15747,10 @@
       </c>
     </row>
     <row r="49" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A49" s="168" t="s">
-        <v>276</v>
-      </c>
-      <c r="B49" s="168"/>
+      <c r="A49" s="172" t="s">
+        <v>272</v>
+      </c>
+      <c r="B49" s="172"/>
       <c r="C49">
         <f t="shared" ref="C49" si="7">C48/5</f>
         <v>0</v>
@@ -16341,7 +16364,7 @@
     </row>
     <row r="52" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished: extract unique extension. Next: calculate suport of extension
</commit_message>
<xml_diff>
--- a/MyThesis.xlsx
+++ b/MyThesis.xlsx
@@ -185,12 +185,108 @@
         </r>
       </text>
     </comment>
+    <comment ref="B47" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Binh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Li = INT(index/(Le*Lv))</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B48" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Binh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+=(i%(Le*Lv))</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B50" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Binh:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>=(i%(Le*Lv))/Lv</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B51" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Binh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+=(i%(Le*Lv)-(((i%(Le*Lv))/Lv)*Lv)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="282">
   <si>
     <t>A</t>
   </si>
@@ -1041,12 +1137,24 @@
   <si>
     <t>scan V: index</t>
   </si>
+  <si>
+    <t>Số lượng mở rộng hợp lệ của một đỉnh: Le*Lv. Còn của mọi đỉnh là: Le*Lv*Lv</t>
+  </si>
+  <si>
+    <t>&lt;--:d_allPossibleExtension</t>
+  </si>
+  <si>
+    <t>&lt;--:d_allPossibleExtensionScanResult</t>
+  </si>
+  <si>
+    <t>&lt;--:d_UniqueExtension</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1159,6 +1267,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="27">
@@ -1821,7 +1935,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2153,6 +2267,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2183,7 +2301,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6452,36 +6569,36 @@
       <c r="B35" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="171" t="s">
+      <c r="C35" s="173" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="166"/>
-      <c r="E35" s="167"/>
-      <c r="F35" s="171" t="s">
+      <c r="D35" s="168"/>
+      <c r="E35" s="169"/>
+      <c r="F35" s="173" t="s">
         <v>74</v>
       </c>
-      <c r="G35" s="166"/>
-      <c r="H35" s="167"/>
-      <c r="I35" s="171" t="s">
+      <c r="G35" s="168"/>
+      <c r="H35" s="169"/>
+      <c r="I35" s="173" t="s">
         <v>80</v>
       </c>
-      <c r="J35" s="166"/>
-      <c r="K35" s="167"/>
-      <c r="L35" s="171" t="s">
+      <c r="J35" s="168"/>
+      <c r="K35" s="169"/>
+      <c r="L35" s="173" t="s">
         <v>82</v>
       </c>
-      <c r="M35" s="166"/>
-      <c r="N35" s="167"/>
-      <c r="O35" s="171" t="s">
+      <c r="M35" s="168"/>
+      <c r="N35" s="169"/>
+      <c r="O35" s="173" t="s">
         <v>84</v>
       </c>
-      <c r="P35" s="166"/>
-      <c r="Q35" s="167"/>
-      <c r="R35" s="165" t="s">
+      <c r="P35" s="168"/>
+      <c r="Q35" s="169"/>
+      <c r="R35" s="167" t="s">
         <v>91</v>
       </c>
-      <c r="S35" s="166"/>
-      <c r="T35" s="167"/>
+      <c r="S35" s="168"/>
+      <c r="T35" s="169"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B36" s="50" t="s">
@@ -6624,16 +6741,16 @@
       <c r="B48" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="168" t="s">
+      <c r="C48" s="170" t="s">
         <v>70</v>
       </c>
-      <c r="D48" s="169"/>
-      <c r="E48" s="170"/>
-      <c r="F48" s="171" t="s">
+      <c r="D48" s="171"/>
+      <c r="E48" s="172"/>
+      <c r="F48" s="173" t="s">
         <v>74</v>
       </c>
-      <c r="G48" s="166"/>
-      <c r="H48" s="167"/>
+      <c r="G48" s="168"/>
+      <c r="H48" s="169"/>
     </row>
     <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" s="33" t="s">
@@ -6998,14 +7115,14 @@
     </row>
     <row r="58" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="163" t="s">
+      <c r="C59" s="165" t="s">
         <v>102</v>
       </c>
-      <c r="D59" s="164"/>
-      <c r="F59" s="163" t="s">
+      <c r="D59" s="166"/>
+      <c r="F59" s="165" t="s">
         <v>103</v>
       </c>
-      <c r="G59" s="164"/>
+      <c r="G59" s="166"/>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B60">
@@ -12157,8 +12274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="AL15" sqref="AL15:AO15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13286,7 +13403,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B17" s="152" t="s">
         <v>262</v>
       </c>
@@ -13297,8 +13414,11 @@
         <f>Li*Lv*Le + Lij*Lv+Lj</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B18" s="152" t="s">
         <v>263</v>
       </c>
@@ -13306,87 +13426,87 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="160" t="s">
         <v>254</v>
       </c>
-      <c r="B19" s="173">
-        <v>0</v>
-      </c>
-      <c r="C19" s="173">
-        <v>1</v>
-      </c>
-      <c r="D19" s="173">
-        <v>2</v>
-      </c>
-      <c r="E19" s="173">
-        <v>3</v>
-      </c>
-      <c r="F19" s="173">
-        <v>4</v>
-      </c>
-      <c r="G19" s="173">
+      <c r="B19" s="163">
+        <v>0</v>
+      </c>
+      <c r="C19" s="163">
+        <v>1</v>
+      </c>
+      <c r="D19" s="163">
+        <v>2</v>
+      </c>
+      <c r="E19" s="163">
+        <v>3</v>
+      </c>
+      <c r="F19" s="163">
+        <v>4</v>
+      </c>
+      <c r="G19" s="163">
         <v>5</v>
       </c>
-      <c r="H19" s="173">
+      <c r="H19" s="163">
         <v>6</v>
       </c>
-      <c r="I19" s="173">
+      <c r="I19" s="163">
         <v>7</v>
       </c>
-      <c r="J19" s="173">
+      <c r="J19" s="163">
         <v>8</v>
       </c>
-      <c r="K19" s="173">
+      <c r="K19" s="163">
         <v>9</v>
       </c>
-      <c r="L19" s="173">
+      <c r="L19" s="163">
         <v>10</v>
       </c>
-      <c r="M19" s="173">
+      <c r="M19" s="163">
         <v>11</v>
       </c>
-      <c r="N19" s="173">
+      <c r="N19" s="163">
         <v>12</v>
       </c>
-      <c r="O19" s="173">
+      <c r="O19" s="163">
         <v>13</v>
       </c>
-      <c r="P19" s="173">
+      <c r="P19" s="163">
         <v>14</v>
       </c>
-      <c r="Q19" s="173">
+      <c r="Q19" s="163">
         <v>15</v>
       </c>
-      <c r="R19" s="173">
+      <c r="R19" s="163">
         <v>16</v>
       </c>
-      <c r="S19" s="173">
+      <c r="S19" s="163">
         <v>17</v>
       </c>
-      <c r="T19" s="173">
+      <c r="T19" s="163">
         <v>18</v>
       </c>
-      <c r="U19" s="173">
+      <c r="U19" s="163">
         <v>19</v>
       </c>
-      <c r="V19" s="173">
+      <c r="V19" s="163">
         <v>20</v>
       </c>
-      <c r="W19" s="173">
+      <c r="W19" s="163">
         <v>21</v>
       </c>
-      <c r="X19" s="173">
+      <c r="X19" s="163">
         <v>22</v>
       </c>
-      <c r="Y19" s="173">
+      <c r="Y19" s="163">
         <v>23</v>
       </c>
-      <c r="Z19" s="173">
+      <c r="Z19" s="163">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:27" s="148" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="154"/>
       <c r="B20" s="148" t="s">
         <v>0</v>
@@ -13464,7 +13584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:27" s="148" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="154"/>
       <c r="B21" s="148" t="s">
         <v>0</v>
@@ -13542,7 +13662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:27" s="148" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="154" t="s">
         <v>257</v>
       </c>
@@ -13622,7 +13742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:27" s="148" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="154" t="s">
         <v>258</v>
       </c>
@@ -13702,7 +13822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:27" s="148" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="154" t="s">
         <v>264</v>
       </c>
@@ -13782,107 +13902,107 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="155" t="s">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A25" s="164" t="s">
         <v>265</v>
       </c>
-      <c r="B25" s="144">
+      <c r="B25" s="163">
         <f>B22*$F$17*$F$18+B24*$F$17+B23</f>
         <v>0</v>
       </c>
-      <c r="C25" s="144">
+      <c r="C25" s="163">
         <f t="shared" ref="C25:Z25" si="2">C22*$F$17*$F$18+C24*$F$17+C23</f>
         <v>1</v>
       </c>
-      <c r="D25" s="144">
+      <c r="D25" s="163">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E25" s="144">
+      <c r="E25" s="163">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="F25" s="144">
+      <c r="F25" s="163">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G25" s="144">
+      <c r="G25" s="163">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H25" s="144">
+      <c r="H25" s="163">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="I25" s="144">
+      <c r="I25" s="163">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="J25" s="144">
+      <c r="J25" s="163">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="K25" s="144">
+      <c r="K25" s="163">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="L25" s="144">
+      <c r="L25" s="163">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="M25" s="144">
+      <c r="M25" s="163">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="N25" s="144">
+      <c r="N25" s="163">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="O25" s="144">
+      <c r="O25" s="163">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="P25" s="144">
+      <c r="P25" s="163">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="Q25" s="144">
+      <c r="Q25" s="163">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="R25" s="144">
+      <c r="R25" s="163">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="S25" s="144">
+      <c r="S25" s="163">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="T25" s="144">
+      <c r="T25" s="163">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="U25" s="144">
+      <c r="U25" s="163">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="V25" s="144">
+      <c r="V25" s="163">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="W25" s="144">
+      <c r="W25" s="163">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="X25" s="144">
+      <c r="X25" s="163">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="Y25" s="144">
+      <c r="Y25" s="163">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="Z25" s="144">
+      <c r="Z25" s="163">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
@@ -13890,7 +14010,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="26" spans="1:27" s="148" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="154" t="s">
         <v>266</v>
       </c>
@@ -13973,8 +14093,11 @@
         <f>SUM(B26:Z26)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB26" s="158" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="156" t="s">
         <v>267</v>
       </c>
@@ -14077,8 +14200,11 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB27" s="158" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="157" t="s">
         <v>254</v>
       </c>
@@ -14104,7 +14230,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="156" t="s">
         <v>268</v>
       </c>
@@ -14131,7 +14257,7 @@
       </c>
       <c r="M29" s="46"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B30" s="148" t="s">
         <v>1</v>
       </c>
@@ -14154,7 +14280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="154" t="s">
         <v>257</v>
       </c>
@@ -14179,8 +14305,11 @@
       <c r="H31" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="J31" s="158" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="154" t="s">
         <v>258</v>
       </c>
@@ -15341,11 +15470,11 @@
         <v>257</v>
       </c>
       <c r="C47">
-        <f t="shared" ref="C47:AZ47" si="5">INT(C45/(5*2))</f>
+        <f>INT(C45/(5*2))</f>
         <v>0</v>
       </c>
       <c r="D47">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D47:AZ47" si="5">INT(D45/(5*2))</f>
         <v>0</v>
       </c>
       <c r="E47">
@@ -15546,11 +15675,11 @@
         <v>271</v>
       </c>
       <c r="C48">
-        <f t="shared" ref="C48:AZ48" si="6">MOD(C45,5*2)</f>
+        <f>MOD(C45,5*2)</f>
         <v>0</v>
       </c>
       <c r="D48">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D48:AZ48" si="6">MOD(D45,5*2)</f>
         <v>1</v>
       </c>
       <c r="E48">
@@ -15747,12 +15876,12 @@
       </c>
     </row>
     <row r="49" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A49" s="172" t="s">
+      <c r="A49" s="174" t="s">
         <v>272</v>
       </c>
-      <c r="B49" s="172"/>
+      <c r="B49" s="174"/>
       <c r="C49">
-        <f t="shared" ref="C49" si="7">C48/5</f>
+        <f>C48/5</f>
         <v>0</v>
       </c>
       <c r="D49">
@@ -15760,95 +15889,95 @@
         <v>0.2</v>
       </c>
       <c r="E49">
-        <f t="shared" ref="E49" si="8">E48/5</f>
+        <f t="shared" ref="E49" si="7">E48/5</f>
         <v>0.4</v>
       </c>
       <c r="F49">
-        <f t="shared" ref="F49" si="9">F48/5</f>
+        <f t="shared" ref="F49" si="8">F48/5</f>
         <v>0.6</v>
       </c>
       <c r="G49">
-        <f t="shared" ref="G49:H49" si="10">G48/5</f>
+        <f t="shared" ref="G49:H49" si="9">G48/5</f>
         <v>0.8</v>
       </c>
       <c r="H49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I49">
-        <f t="shared" ref="I49" si="11">I48/5</f>
+        <f t="shared" ref="I49" si="10">I48/5</f>
         <v>1.2</v>
       </c>
       <c r="J49">
-        <f t="shared" ref="J49" si="12">J48/5</f>
+        <f t="shared" ref="J49" si="11">J48/5</f>
         <v>1.4</v>
       </c>
       <c r="K49">
-        <f t="shared" ref="K49" si="13">K48/5</f>
+        <f t="shared" ref="K49" si="12">K48/5</f>
         <v>1.6</v>
       </c>
       <c r="L49">
-        <f t="shared" ref="L49" si="14">L48/5</f>
+        <f t="shared" ref="L49" si="13">L48/5</f>
         <v>1.8</v>
       </c>
       <c r="M49">
-        <f t="shared" ref="M49" si="15">M48/5</f>
+        <f t="shared" ref="M49" si="14">M48/5</f>
         <v>0</v>
       </c>
       <c r="N49">
-        <f t="shared" ref="N49" si="16">N48/5</f>
+        <f t="shared" ref="N49" si="15">N48/5</f>
         <v>0.2</v>
       </c>
       <c r="O49">
-        <f t="shared" ref="O49" si="17">O48/5</f>
+        <f t="shared" ref="O49" si="16">O48/5</f>
         <v>0.4</v>
       </c>
       <c r="P49">
-        <f t="shared" ref="P49" si="18">P48/5</f>
+        <f t="shared" ref="P49" si="17">P48/5</f>
         <v>0.6</v>
       </c>
       <c r="Q49">
-        <f t="shared" ref="Q49:R49" si="19">Q48/5</f>
+        <f t="shared" ref="Q49:R49" si="18">Q48/5</f>
         <v>0.8</v>
       </c>
       <c r="R49">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="S49">
-        <f t="shared" ref="S49" si="20">S48/5</f>
+        <f t="shared" ref="S49" si="19">S48/5</f>
         <v>1.2</v>
       </c>
       <c r="T49">
-        <f t="shared" ref="T49" si="21">T48/5</f>
+        <f t="shared" ref="T49" si="20">T48/5</f>
         <v>1.4</v>
       </c>
       <c r="U49">
-        <f t="shared" ref="U49" si="22">U48/5</f>
+        <f t="shared" ref="U49" si="21">U48/5</f>
         <v>1.6</v>
       </c>
       <c r="V49">
-        <f t="shared" ref="V49" si="23">V48/5</f>
+        <f t="shared" ref="V49" si="22">V48/5</f>
         <v>1.8</v>
       </c>
       <c r="W49">
-        <f t="shared" ref="W49:AA49" si="24">W48/5</f>
+        <f t="shared" ref="W49:AA49" si="23">W48/5</f>
         <v>0</v>
       </c>
       <c r="X49">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.2</v>
       </c>
       <c r="Y49">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.4</v>
       </c>
       <c r="Z49">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.6</v>
       </c>
       <c r="AA49">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.8</v>
       </c>
       <c r="AB49">
@@ -15856,99 +15985,99 @@
         <v>1</v>
       </c>
       <c r="AC49">
-        <f t="shared" ref="AC49:AF49" si="25">AC48/5</f>
+        <f t="shared" ref="AC49:AF49" si="24">AC48/5</f>
         <v>1.2</v>
       </c>
       <c r="AD49">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>1.4</v>
       </c>
       <c r="AE49">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>1.6</v>
       </c>
       <c r="AF49">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>1.8</v>
       </c>
       <c r="AG49">
-        <f t="shared" ref="AG49" si="26">AG48/5</f>
+        <f t="shared" ref="AG49" si="25">AG48/5</f>
         <v>0</v>
       </c>
       <c r="AH49">
-        <f t="shared" ref="AH49" si="27">AH48/5</f>
+        <f t="shared" ref="AH49" si="26">AH48/5</f>
         <v>0.2</v>
       </c>
       <c r="AI49">
-        <f t="shared" ref="AI49" si="28">AI48/5</f>
+        <f t="shared" ref="AI49" si="27">AI48/5</f>
         <v>0.4</v>
       </c>
       <c r="AJ49">
-        <f t="shared" ref="AJ49" si="29">AJ48/5</f>
+        <f t="shared" ref="AJ49" si="28">AJ48/5</f>
         <v>0.6</v>
       </c>
       <c r="AK49">
-        <f t="shared" ref="AK49" si="30">AK48/5</f>
+        <f t="shared" ref="AK49" si="29">AK48/5</f>
         <v>0.8</v>
       </c>
       <c r="AL49">
-        <f t="shared" ref="AL49" si="31">AL48/5</f>
+        <f t="shared" ref="AL49" si="30">AL48/5</f>
         <v>1</v>
       </c>
       <c r="AM49">
-        <f t="shared" ref="AM49" si="32">AM48/5</f>
+        <f t="shared" ref="AM49" si="31">AM48/5</f>
         <v>1.2</v>
       </c>
       <c r="AN49">
-        <f t="shared" ref="AN49" si="33">AN48/5</f>
+        <f t="shared" ref="AN49" si="32">AN48/5</f>
         <v>1.4</v>
       </c>
       <c r="AO49">
-        <f t="shared" ref="AO49" si="34">AO48/5</f>
+        <f t="shared" ref="AO49" si="33">AO48/5</f>
         <v>1.6</v>
       </c>
       <c r="AP49">
-        <f t="shared" ref="AP49" si="35">AP48/5</f>
+        <f t="shared" ref="AP49" si="34">AP48/5</f>
         <v>1.8</v>
       </c>
       <c r="AQ49">
-        <f t="shared" ref="AQ49" si="36">AQ48/5</f>
+        <f t="shared" ref="AQ49" si="35">AQ48/5</f>
         <v>0</v>
       </c>
       <c r="AR49">
-        <f t="shared" ref="AR49" si="37">AR48/5</f>
+        <f t="shared" ref="AR49" si="36">AR48/5</f>
         <v>0.2</v>
       </c>
       <c r="AS49">
-        <f t="shared" ref="AS49" si="38">AS48/5</f>
+        <f t="shared" ref="AS49" si="37">AS48/5</f>
         <v>0.4</v>
       </c>
       <c r="AT49">
-        <f t="shared" ref="AT49" si="39">AT48/5</f>
+        <f t="shared" ref="AT49" si="38">AT48/5</f>
         <v>0.6</v>
       </c>
       <c r="AU49">
-        <f t="shared" ref="AU49" si="40">AU48/5</f>
+        <f t="shared" ref="AU49" si="39">AU48/5</f>
         <v>0.8</v>
       </c>
       <c r="AV49">
-        <f t="shared" ref="AV49" si="41">AV48/5</f>
+        <f t="shared" ref="AV49" si="40">AV48/5</f>
         <v>1</v>
       </c>
       <c r="AW49">
-        <f t="shared" ref="AW49" si="42">AW48/5</f>
+        <f t="shared" ref="AW49" si="41">AW48/5</f>
         <v>1.2</v>
       </c>
       <c r="AX49">
-        <f t="shared" ref="AX49" si="43">AX48/5</f>
+        <f t="shared" ref="AX49" si="42">AX48/5</f>
         <v>1.4</v>
       </c>
       <c r="AY49">
-        <f t="shared" ref="AY49" si="44">AY48/5</f>
+        <f t="shared" ref="AY49" si="43">AY48/5</f>
         <v>1.6</v>
       </c>
       <c r="AZ49">
-        <f t="shared" ref="AZ49" si="45">AZ48/5</f>
+        <f t="shared" ref="AZ49" si="44">AZ48/5</f>
         <v>1.8</v>
       </c>
     </row>
@@ -15957,83 +16086,83 @@
         <v>138</v>
       </c>
       <c r="C50">
-        <f t="shared" ref="C50" si="46">INT(C49)</f>
+        <f>INT(C49)</f>
         <v>0</v>
       </c>
       <c r="D50">
-        <f t="shared" ref="D50" si="47">INT(D49)</f>
+        <f t="shared" ref="D50" si="45">INT(D49)</f>
         <v>0</v>
       </c>
       <c r="E50">
-        <f t="shared" ref="E50" si="48">INT(E49)</f>
+        <f t="shared" ref="E50" si="46">INT(E49)</f>
         <v>0</v>
       </c>
       <c r="F50">
-        <f t="shared" ref="F50" si="49">INT(F49)</f>
+        <f t="shared" ref="F50" si="47">INT(F49)</f>
         <v>0</v>
       </c>
       <c r="G50">
-        <f t="shared" ref="G50" si="50">INT(G49)</f>
+        <f t="shared" ref="G50" si="48">INT(G49)</f>
         <v>0</v>
       </c>
       <c r="H50">
-        <f t="shared" ref="H50" si="51">INT(H49)</f>
+        <f t="shared" ref="H50" si="49">INT(H49)</f>
         <v>1</v>
       </c>
       <c r="I50">
-        <f t="shared" ref="I50" si="52">INT(I49)</f>
+        <f t="shared" ref="I50" si="50">INT(I49)</f>
         <v>1</v>
       </c>
       <c r="J50">
-        <f t="shared" ref="J50" si="53">INT(J49)</f>
+        <f t="shared" ref="J50" si="51">INT(J49)</f>
         <v>1</v>
       </c>
       <c r="K50">
-        <f t="shared" ref="K50" si="54">INT(K49)</f>
+        <f t="shared" ref="K50" si="52">INT(K49)</f>
         <v>1</v>
       </c>
       <c r="L50">
-        <f t="shared" ref="L50:M50" si="55">INT(L49)</f>
+        <f t="shared" ref="L50:M50" si="53">INT(L49)</f>
         <v>1</v>
       </c>
       <c r="M50">
-        <f t="shared" si="55"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="N50">
-        <f t="shared" ref="N50" si="56">INT(N49)</f>
+        <f t="shared" ref="N50" si="54">INT(N49)</f>
         <v>0</v>
       </c>
       <c r="O50">
-        <f t="shared" ref="O50" si="57">INT(O49)</f>
+        <f t="shared" ref="O50" si="55">INT(O49)</f>
         <v>0</v>
       </c>
       <c r="P50">
-        <f t="shared" ref="P50" si="58">INT(P49)</f>
+        <f t="shared" ref="P50" si="56">INT(P49)</f>
         <v>0</v>
       </c>
       <c r="Q50">
-        <f t="shared" ref="Q50" si="59">INT(Q49)</f>
+        <f t="shared" ref="Q50" si="57">INT(Q49)</f>
         <v>0</v>
       </c>
       <c r="R50">
-        <f t="shared" ref="R50" si="60">INT(R49)</f>
+        <f t="shared" ref="R50" si="58">INT(R49)</f>
         <v>1</v>
       </c>
       <c r="S50">
-        <f t="shared" ref="S50" si="61">INT(S49)</f>
+        <f t="shared" ref="S50" si="59">INT(S49)</f>
         <v>1</v>
       </c>
       <c r="T50">
-        <f t="shared" ref="T50" si="62">INT(T49)</f>
+        <f t="shared" ref="T50" si="60">INT(T49)</f>
         <v>1</v>
       </c>
       <c r="U50">
-        <f t="shared" ref="U50" si="63">INT(U49)</f>
+        <f t="shared" ref="U50" si="61">INT(U49)</f>
         <v>1</v>
       </c>
       <c r="V50">
-        <f t="shared" ref="V50" si="64">INT(V49)</f>
+        <f t="shared" ref="V50" si="62">INT(V49)</f>
         <v>1</v>
       </c>
       <c r="W50">
@@ -16041,119 +16170,119 @@
         <v>0</v>
       </c>
       <c r="X50">
-        <f t="shared" ref="X50:AF50" si="65">INT(X49)</f>
+        <f t="shared" ref="X50:AF50" si="63">INT(X49)</f>
         <v>0</v>
       </c>
       <c r="Y50">
-        <f t="shared" si="65"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="Z50">
-        <f t="shared" si="65"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AA50">
-        <f t="shared" si="65"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AB50">
-        <f t="shared" si="65"/>
+        <f t="shared" si="63"/>
         <v>1</v>
       </c>
       <c r="AC50">
-        <f t="shared" si="65"/>
+        <f t="shared" si="63"/>
         <v>1</v>
       </c>
       <c r="AD50">
-        <f t="shared" si="65"/>
+        <f t="shared" si="63"/>
         <v>1</v>
       </c>
       <c r="AE50">
-        <f t="shared" si="65"/>
+        <f t="shared" si="63"/>
         <v>1</v>
       </c>
       <c r="AF50">
-        <f t="shared" si="65"/>
+        <f t="shared" si="63"/>
         <v>1</v>
       </c>
       <c r="AG50">
-        <f t="shared" ref="AG50" si="66">INT(AG49)</f>
+        <f t="shared" ref="AG50" si="64">INT(AG49)</f>
         <v>0</v>
       </c>
       <c r="AH50">
-        <f t="shared" ref="AH50" si="67">INT(AH49)</f>
+        <f t="shared" ref="AH50" si="65">INT(AH49)</f>
         <v>0</v>
       </c>
       <c r="AI50">
-        <f t="shared" ref="AI50" si="68">INT(AI49)</f>
+        <f t="shared" ref="AI50" si="66">INT(AI49)</f>
         <v>0</v>
       </c>
       <c r="AJ50">
-        <f t="shared" ref="AJ50" si="69">INT(AJ49)</f>
+        <f t="shared" ref="AJ50" si="67">INT(AJ49)</f>
         <v>0</v>
       </c>
       <c r="AK50">
-        <f t="shared" ref="AK50" si="70">INT(AK49)</f>
+        <f t="shared" ref="AK50" si="68">INT(AK49)</f>
         <v>0</v>
       </c>
       <c r="AL50">
-        <f t="shared" ref="AL50" si="71">INT(AL49)</f>
+        <f t="shared" ref="AL50" si="69">INT(AL49)</f>
         <v>1</v>
       </c>
       <c r="AM50">
-        <f t="shared" ref="AM50" si="72">INT(AM49)</f>
+        <f t="shared" ref="AM50" si="70">INT(AM49)</f>
         <v>1</v>
       </c>
       <c r="AN50">
-        <f t="shared" ref="AN50" si="73">INT(AN49)</f>
+        <f t="shared" ref="AN50" si="71">INT(AN49)</f>
         <v>1</v>
       </c>
       <c r="AO50">
-        <f t="shared" ref="AO50" si="74">INT(AO49)</f>
+        <f t="shared" ref="AO50" si="72">INT(AO49)</f>
         <v>1</v>
       </c>
       <c r="AP50">
-        <f t="shared" ref="AP50" si="75">INT(AP49)</f>
+        <f t="shared" ref="AP50" si="73">INT(AP49)</f>
         <v>1</v>
       </c>
       <c r="AQ50">
-        <f t="shared" ref="AQ50" si="76">INT(AQ49)</f>
+        <f t="shared" ref="AQ50" si="74">INT(AQ49)</f>
         <v>0</v>
       </c>
       <c r="AR50">
-        <f t="shared" ref="AR50" si="77">INT(AR49)</f>
+        <f t="shared" ref="AR50" si="75">INT(AR49)</f>
         <v>0</v>
       </c>
       <c r="AS50">
-        <f t="shared" ref="AS50" si="78">INT(AS49)</f>
+        <f t="shared" ref="AS50" si="76">INT(AS49)</f>
         <v>0</v>
       </c>
       <c r="AT50">
-        <f t="shared" ref="AT50" si="79">INT(AT49)</f>
+        <f t="shared" ref="AT50" si="77">INT(AT49)</f>
         <v>0</v>
       </c>
       <c r="AU50">
-        <f t="shared" ref="AU50" si="80">INT(AU49)</f>
+        <f t="shared" ref="AU50" si="78">INT(AU49)</f>
         <v>0</v>
       </c>
       <c r="AV50">
-        <f t="shared" ref="AV50" si="81">INT(AV49)</f>
+        <f t="shared" ref="AV50" si="79">INT(AV49)</f>
         <v>1</v>
       </c>
       <c r="AW50">
-        <f t="shared" ref="AW50" si="82">INT(AW49)</f>
+        <f t="shared" ref="AW50" si="80">INT(AW49)</f>
         <v>1</v>
       </c>
       <c r="AX50">
-        <f t="shared" ref="AX50" si="83">INT(AX49)</f>
+        <f t="shared" ref="AX50" si="81">INT(AX49)</f>
         <v>1</v>
       </c>
       <c r="AY50">
-        <f t="shared" ref="AY50" si="84">INT(AY49)</f>
+        <f t="shared" ref="AY50" si="82">INT(AY49)</f>
         <v>1</v>
       </c>
       <c r="AZ50">
-        <f t="shared" ref="AZ50" si="85">INT(AZ49)</f>
+        <f t="shared" ref="AZ50" si="83">INT(AZ49)</f>
         <v>1</v>
       </c>
     </row>
@@ -16162,63 +16291,63 @@
         <v>137</v>
       </c>
       <c r="C51">
-        <f t="shared" ref="C51:Q51" si="86">C48-(C50*5)</f>
+        <f>C48-(C50*5)</f>
         <v>0</v>
       </c>
       <c r="D51">
-        <f t="shared" si="86"/>
+        <f t="shared" ref="C51:Q51" si="84">D48-(D50*5)</f>
         <v>1</v>
       </c>
       <c r="E51">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>2</v>
       </c>
       <c r="F51">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>3</v>
       </c>
       <c r="G51">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>4</v>
       </c>
       <c r="H51">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="I51">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>1</v>
       </c>
       <c r="J51">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>2</v>
       </c>
       <c r="K51">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>3</v>
       </c>
       <c r="L51">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>4</v>
       </c>
       <c r="M51">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="N51">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>1</v>
       </c>
       <c r="O51">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>2</v>
       </c>
       <c r="P51">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>3</v>
       </c>
       <c r="Q51">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>4</v>
       </c>
       <c r="R51">
@@ -16226,15 +16355,15 @@
         <v>0</v>
       </c>
       <c r="S51">
-        <f t="shared" ref="S51:U51" si="87">S48-(S50*5)</f>
+        <f t="shared" ref="S51:U51" si="85">S48-(S50*5)</f>
         <v>1</v>
       </c>
       <c r="T51">
-        <f t="shared" si="87"/>
+        <f t="shared" si="85"/>
         <v>2</v>
       </c>
       <c r="U51">
-        <f t="shared" si="87"/>
+        <f t="shared" si="85"/>
         <v>3</v>
       </c>
       <c r="V51">
@@ -16242,123 +16371,123 @@
         <v>4</v>
       </c>
       <c r="W51">
-        <f t="shared" ref="W51" si="88">W48-(W50*5)</f>
+        <f t="shared" ref="W51" si="86">W48-(W50*5)</f>
         <v>0</v>
       </c>
       <c r="X51">
-        <f t="shared" ref="X51" si="89">X48-(X50*5)</f>
+        <f t="shared" ref="X51" si="87">X48-(X50*5)</f>
         <v>1</v>
       </c>
       <c r="Y51">
-        <f t="shared" ref="Y51" si="90">Y48-(Y50*5)</f>
+        <f t="shared" ref="Y51" si="88">Y48-(Y50*5)</f>
         <v>2</v>
       </c>
       <c r="Z51">
-        <f t="shared" ref="Z51:AB51" si="91">Z48-(Z50*5)</f>
+        <f t="shared" ref="Z51:AB51" si="89">Z48-(Z50*5)</f>
         <v>3</v>
       </c>
       <c r="AA51">
-        <f t="shared" si="91"/>
+        <f t="shared" si="89"/>
         <v>4</v>
       </c>
       <c r="AB51">
-        <f t="shared" si="91"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="AC51">
-        <f t="shared" ref="AC51" si="92">AC48-(AC50*5)</f>
+        <f t="shared" ref="AC51" si="90">AC48-(AC50*5)</f>
         <v>1</v>
       </c>
       <c r="AD51">
-        <f t="shared" ref="AD51" si="93">AD48-(AD50*5)</f>
+        <f t="shared" ref="AD51" si="91">AD48-(AD50*5)</f>
         <v>2</v>
       </c>
       <c r="AE51">
-        <f t="shared" ref="AE51:AG51" si="94">AE48-(AE50*5)</f>
+        <f t="shared" ref="AE51:AG51" si="92">AE48-(AE50*5)</f>
         <v>3</v>
       </c>
       <c r="AF51">
-        <f t="shared" si="94"/>
+        <f t="shared" si="92"/>
         <v>4</v>
       </c>
       <c r="AG51">
-        <f t="shared" si="94"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AH51">
-        <f t="shared" ref="AH51" si="95">AH48-(AH50*5)</f>
+        <f t="shared" ref="AH51" si="93">AH48-(AH50*5)</f>
         <v>1</v>
       </c>
       <c r="AI51">
-        <f t="shared" ref="AI51" si="96">AI48-(AI50*5)</f>
+        <f t="shared" ref="AI51" si="94">AI48-(AI50*5)</f>
         <v>2</v>
       </c>
       <c r="AJ51">
-        <f t="shared" ref="AJ51:AL51" si="97">AJ48-(AJ50*5)</f>
+        <f t="shared" ref="AJ51:AL51" si="95">AJ48-(AJ50*5)</f>
         <v>3</v>
       </c>
       <c r="AK51">
-        <f t="shared" si="97"/>
+        <f t="shared" si="95"/>
         <v>4</v>
       </c>
       <c r="AL51">
-        <f t="shared" si="97"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="AM51">
-        <f t="shared" ref="AM51" si="98">AM48-(AM50*5)</f>
+        <f t="shared" ref="AM51" si="96">AM48-(AM50*5)</f>
         <v>1</v>
       </c>
       <c r="AN51">
-        <f t="shared" ref="AN51" si="99">AN48-(AN50*5)</f>
+        <f t="shared" ref="AN51" si="97">AN48-(AN50*5)</f>
         <v>2</v>
       </c>
       <c r="AO51">
-        <f t="shared" ref="AO51:AQ51" si="100">AO48-(AO50*5)</f>
+        <f t="shared" ref="AO51:AQ51" si="98">AO48-(AO50*5)</f>
         <v>3</v>
       </c>
       <c r="AP51">
-        <f t="shared" si="100"/>
+        <f t="shared" si="98"/>
         <v>4</v>
       </c>
       <c r="AQ51">
-        <f t="shared" si="100"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="AR51">
-        <f t="shared" ref="AR51" si="101">AR48-(AR50*5)</f>
+        <f t="shared" ref="AR51" si="99">AR48-(AR50*5)</f>
         <v>1</v>
       </c>
       <c r="AS51">
-        <f t="shared" ref="AS51" si="102">AS48-(AS50*5)</f>
+        <f t="shared" ref="AS51" si="100">AS48-(AS50*5)</f>
         <v>2</v>
       </c>
       <c r="AT51">
-        <f t="shared" ref="AT51:AV51" si="103">AT48-(AT50*5)</f>
+        <f t="shared" ref="AT51:AV51" si="101">AT48-(AT50*5)</f>
         <v>3</v>
       </c>
       <c r="AU51">
-        <f t="shared" si="103"/>
+        <f t="shared" si="101"/>
         <v>4</v>
       </c>
       <c r="AV51">
-        <f t="shared" si="103"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="AW51">
-        <f t="shared" ref="AW51" si="104">AW48-(AW50*5)</f>
+        <f t="shared" ref="AW51" si="102">AW48-(AW50*5)</f>
         <v>1</v>
       </c>
       <c r="AX51">
-        <f t="shared" ref="AX51" si="105">AX48-(AX50*5)</f>
+        <f t="shared" ref="AX51" si="103">AX48-(AX50*5)</f>
         <v>2</v>
       </c>
       <c r="AY51">
-        <f t="shared" ref="AY51:AZ51" si="106">AY48-(AY50*5)</f>
+        <f t="shared" ref="AY51:AZ51" si="104">AY48-(AY50*5)</f>
         <v>3</v>
       </c>
       <c r="AZ51">
-        <f t="shared" si="106"/>
+        <f t="shared" si="104"/>
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished: we got array F for each unique extension. Next: reduction F to get support for them
</commit_message>
<xml_diff>
--- a/MyThesis.xlsx
+++ b/MyThesis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6870" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6870" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="ScanLargeArray" sheetId="7" r:id="rId6"/>
     <sheet name="GlobalMemoryRead" sheetId="8" r:id="rId7"/>
     <sheet name="ExtractUniqueExtension" sheetId="9" r:id="rId8"/>
+    <sheet name="ComputeSupport" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="Le">'Extraction of Unique Edge'!$C$3</definedName>
@@ -285,8 +286,115 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>BinhTruong</author>
+    <author>Bencat</author>
+  </authors>
+  <commentList>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>BinhTruong:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mảng B có số lượng phần tử bằng với d_validExtension</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Bình:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Công thức được tính bằng: graphId phía sau trừ cho graph id đang xét.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q7" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Binh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Giá trị cuối của mảng B luôn là zero, vì phía sau nó không giáp với đồ thị nào ở phía sau.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>BinhTruong:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mảng unsinged int *F có số lượng phần tử bằng với kết quả của phần tử cuối cùng của ScanB cộng cho 1 (2+1=3)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="288">
   <si>
     <t>A</t>
   </si>
@@ -1149,12 +1257,30 @@
   <si>
     <t>&lt;--:d_UniqueExtension</t>
   </si>
+  <si>
+    <t>ScanB</t>
+  </si>
+  <si>
+    <t>F index</t>
+  </si>
+  <si>
+    <t>&lt;&lt;===|Ví dụ tính Support cho cạnh AB</t>
+  </si>
+  <si>
+    <t>Reduce F</t>
+  </si>
+  <si>
+    <t>Array d_F</t>
+  </si>
+  <si>
+    <t>Array d_B</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1274,8 +1400,15 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="27">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1429,6 +1562,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1935,7 +2074,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2271,6 +2410,19 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2305,7 +2457,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3881,16 +4043,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3914,7 +4076,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6153150" y="2009775"/>
+          <a:off x="6934200" y="1895475"/>
           <a:ext cx="3705225" cy="819150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3930,6 +4092,233 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>198755</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>8255</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5629275" y="5219700"/>
+          <a:ext cx="5732780" cy="2027555"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1028699</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5457825" cy="923458"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028699" y="3419475"/>
+          <a:ext cx="5457825" cy="923458"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="vi-VN" sz="1100"/>
+            <a:t>Tương ứng với mỗi mở rộng duy nhất trong d_UniqueExtension, chúng ta tạo ra số lượng thread i bằng số với số lượng phần tử của mảng d_ValidExtension, nếu Li và Lj trong d_ValidExtension</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="vi-VN" sz="1100"/>
+            <a:t>bằng với Li và Lj của mở rộng đang xét thì sẽ gán giá trị là 1 tại vị trí F[ScanB[i]]. Cuối cùng chúng ta thực hiện reduction trên mảng F để có được kết quả độ hỗ trợ cho mở rộng.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>180209</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>180908</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7962900" y="1933575"/>
+          <a:ext cx="6123809" cy="533333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>513586</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>190435</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7696200" y="2714625"/>
+          <a:ext cx="6114286" cy="523810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571187</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>37975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7705725" y="3419475"/>
+          <a:ext cx="2504762" cy="1000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -6266,10 +6655,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K18:K53">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6569,36 +6958,36 @@
       <c r="B35" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="173" t="s">
+      <c r="C35" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="168"/>
-      <c r="E35" s="169"/>
-      <c r="F35" s="173" t="s">
+      <c r="D35" s="173"/>
+      <c r="E35" s="174"/>
+      <c r="F35" s="178" t="s">
         <v>74</v>
       </c>
-      <c r="G35" s="168"/>
-      <c r="H35" s="169"/>
-      <c r="I35" s="173" t="s">
+      <c r="G35" s="173"/>
+      <c r="H35" s="174"/>
+      <c r="I35" s="178" t="s">
         <v>80</v>
       </c>
-      <c r="J35" s="168"/>
-      <c r="K35" s="169"/>
-      <c r="L35" s="173" t="s">
+      <c r="J35" s="173"/>
+      <c r="K35" s="174"/>
+      <c r="L35" s="178" t="s">
         <v>82</v>
       </c>
-      <c r="M35" s="168"/>
-      <c r="N35" s="169"/>
-      <c r="O35" s="173" t="s">
+      <c r="M35" s="173"/>
+      <c r="N35" s="174"/>
+      <c r="O35" s="178" t="s">
         <v>84</v>
       </c>
-      <c r="P35" s="168"/>
-      <c r="Q35" s="169"/>
-      <c r="R35" s="167" t="s">
+      <c r="P35" s="173"/>
+      <c r="Q35" s="174"/>
+      <c r="R35" s="172" t="s">
         <v>91</v>
       </c>
-      <c r="S35" s="168"/>
-      <c r="T35" s="169"/>
+      <c r="S35" s="173"/>
+      <c r="T35" s="174"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B36" s="50" t="s">
@@ -6741,16 +7130,16 @@
       <c r="B48" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="170" t="s">
+      <c r="C48" s="175" t="s">
         <v>70</v>
       </c>
-      <c r="D48" s="171"/>
-      <c r="E48" s="172"/>
-      <c r="F48" s="173" t="s">
+      <c r="D48" s="176"/>
+      <c r="E48" s="177"/>
+      <c r="F48" s="178" t="s">
         <v>74</v>
       </c>
-      <c r="G48" s="168"/>
-      <c r="H48" s="169"/>
+      <c r="G48" s="173"/>
+      <c r="H48" s="174"/>
     </row>
     <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" s="33" t="s">
@@ -7115,14 +7504,14 @@
     </row>
     <row r="58" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="165" t="s">
+      <c r="C59" s="170" t="s">
         <v>102</v>
       </c>
-      <c r="D59" s="166"/>
-      <c r="F59" s="165" t="s">
+      <c r="D59" s="171"/>
+      <c r="F59" s="170" t="s">
         <v>103</v>
       </c>
-      <c r="G59" s="166"/>
+      <c r="G59" s="171"/>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B60">
@@ -12012,7 +12401,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B7:AG7 B9:AG9">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>B$7&lt;&gt;B$9</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12274,8 +12663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15876,10 +16265,10 @@
       </c>
     </row>
     <row r="49" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A49" s="174" t="s">
+      <c r="A49" s="179" t="s">
         <v>272</v>
       </c>
-      <c r="B49" s="174"/>
+      <c r="B49" s="179"/>
       <c r="C49">
         <f>C48/5</f>
         <v>0</v>
@@ -16295,7 +16684,7 @@
         <v>0</v>
       </c>
       <c r="D51">
-        <f t="shared" ref="C51:Q51" si="84">D48-(D50*5)</f>
+        <f t="shared" ref="D51:Q51" si="84">D48-(D50*5)</f>
         <v>1</v>
       </c>
       <c r="E51">
@@ -16501,21 +16890,657 @@
     <mergeCell ref="A49:B49"/>
   </mergeCells>
   <conditionalFormatting sqref="B8:B9 D9 F9 H9 J9 L9 N9 P9 B15:Q15 B17:B18 B34:H34 B7:AG7">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:Z26 B27">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:B37">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="159" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="149">
+        <v>0</v>
+      </c>
+      <c r="C1" s="162">
+        <v>1</v>
+      </c>
+      <c r="D1" s="149">
+        <v>2</v>
+      </c>
+      <c r="E1" s="162">
+        <v>3</v>
+      </c>
+      <c r="F1" s="149">
+        <v>4</v>
+      </c>
+      <c r="G1" s="162">
+        <v>5</v>
+      </c>
+      <c r="H1" s="149">
+        <v>6</v>
+      </c>
+      <c r="I1" s="162">
+        <v>7</v>
+      </c>
+      <c r="J1" s="149">
+        <v>8</v>
+      </c>
+      <c r="K1" s="162">
+        <v>9</v>
+      </c>
+      <c r="L1" s="149">
+        <v>10</v>
+      </c>
+      <c r="M1" s="162">
+        <v>11</v>
+      </c>
+      <c r="N1" s="149">
+        <v>12</v>
+      </c>
+      <c r="O1" s="162">
+        <v>13</v>
+      </c>
+      <c r="P1" s="149">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="162">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="153" t="s">
+        <v>274</v>
+      </c>
+      <c r="B2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="154" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" s="26">
+        <v>0</v>
+      </c>
+      <c r="C3" s="26">
+        <v>0</v>
+      </c>
+      <c r="D3" s="26">
+        <v>1</v>
+      </c>
+      <c r="E3" s="26">
+        <v>1</v>
+      </c>
+      <c r="F3" s="26">
+        <v>2</v>
+      </c>
+      <c r="G3" s="26">
+        <v>2</v>
+      </c>
+      <c r="H3" s="26">
+        <v>5</v>
+      </c>
+      <c r="I3" s="26">
+        <v>5</v>
+      </c>
+      <c r="J3" s="26">
+        <v>6</v>
+      </c>
+      <c r="K3" s="26">
+        <v>6</v>
+      </c>
+      <c r="L3" s="26">
+        <v>7</v>
+      </c>
+      <c r="M3" s="26">
+        <v>10</v>
+      </c>
+      <c r="N3" s="26">
+        <v>10</v>
+      </c>
+      <c r="O3" s="26">
+        <v>13</v>
+      </c>
+      <c r="P3" s="26">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="154" t="s">
+        <v>256</v>
+      </c>
+      <c r="B4" s="26">
+        <v>1</v>
+      </c>
+      <c r="C4" s="26">
+        <v>2</v>
+      </c>
+      <c r="D4" s="26">
+        <v>3</v>
+      </c>
+      <c r="E4" s="26">
+        <v>4</v>
+      </c>
+      <c r="F4" s="26">
+        <v>3</v>
+      </c>
+      <c r="G4" s="26">
+        <v>4</v>
+      </c>
+      <c r="H4" s="26">
+        <v>6</v>
+      </c>
+      <c r="I4" s="26">
+        <v>7</v>
+      </c>
+      <c r="J4" s="26">
+        <v>7</v>
+      </c>
+      <c r="K4" s="26">
+        <v>8</v>
+      </c>
+      <c r="L4" s="26">
+        <v>9</v>
+      </c>
+      <c r="M4" s="26">
+        <v>11</v>
+      </c>
+      <c r="N4" s="26">
+        <v>12</v>
+      </c>
+      <c r="O4" s="26">
+        <v>10</v>
+      </c>
+      <c r="P4" s="26">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="154" t="s">
+        <v>257</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="154" t="s">
+        <v>258</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="155" t="s">
+        <v>287</v>
+      </c>
+      <c r="B7" s="148">
+        <f>INT(C3/5)-INT(B3/5)</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="148">
+        <f t="shared" ref="C7:P7" si="0">INT(D3/5)-INT(C3/5)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="148">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="148">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="148">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="148">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="148">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="148">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="148">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="148">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="148">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M7" s="148">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="148">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="148">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="148">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="156" t="s">
+        <v>282</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f>B8+B7</f>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:Q8" si="1">C8+C7</f>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="165" t="s">
+        <v>283</v>
+      </c>
+      <c r="B9" s="166">
+        <v>0</v>
+      </c>
+      <c r="C9" s="166">
+        <v>1</v>
+      </c>
+      <c r="D9" s="166">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="157" t="s">
+        <v>286</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="126" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="169" t="s">
+        <v>285</v>
+      </c>
+      <c r="B11" s="168">
+        <f>SUM(B10:D10)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="157" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12" s="151">
+        <v>0</v>
+      </c>
+      <c r="C12" s="151">
+        <v>1</v>
+      </c>
+      <c r="D12" s="151">
+        <v>2</v>
+      </c>
+      <c r="E12" s="151">
+        <v>3</v>
+      </c>
+      <c r="F12" s="151">
+        <v>4</v>
+      </c>
+      <c r="G12" s="151">
+        <v>5</v>
+      </c>
+      <c r="H12" s="151">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="156" t="s">
+        <v>268</v>
+      </c>
+      <c r="B13" s="148" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="148" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="148" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="148" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="148" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="148" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="148" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="46"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="159"/>
+      <c r="B14" s="148" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="148" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="148" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="148" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="148" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="148" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="148" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="154" t="s">
+        <v>257</v>
+      </c>
+      <c r="B15" s="26">
+        <v>0</v>
+      </c>
+      <c r="C15" s="26">
+        <v>0</v>
+      </c>
+      <c r="D15" s="26">
+        <v>0</v>
+      </c>
+      <c r="E15" s="26">
+        <v>1</v>
+      </c>
+      <c r="F15" s="26">
+        <v>1</v>
+      </c>
+      <c r="G15" s="26">
+        <v>1</v>
+      </c>
+      <c r="H15" s="26">
+        <v>2</v>
+      </c>
+      <c r="J15" s="158" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="154" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16" s="26">
+        <v>1</v>
+      </c>
+      <c r="C16" s="26">
+        <v>2</v>
+      </c>
+      <c r="D16" s="26">
+        <v>4</v>
+      </c>
+      <c r="E16" s="26">
+        <v>2</v>
+      </c>
+      <c r="F16" s="26">
+        <v>3</v>
+      </c>
+      <c r="G16" s="26">
+        <v>4</v>
+      </c>
+      <c r="H16" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="B17" s="26">
+        <v>0</v>
+      </c>
+      <c r="C17" s="26">
+        <v>0</v>
+      </c>
+      <c r="D17" s="26">
+        <v>0</v>
+      </c>
+      <c r="E17" s="26">
+        <v>0</v>
+      </c>
+      <c r="F17" s="26">
+        <v>0</v>
+      </c>
+      <c r="G17" s="26">
+        <v>0</v>
+      </c>
+      <c r="H17" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="167"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1 D1 F1 H1 J1 L1 N1 P1 B7:Q7">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
finish:computeboundary Next:ComputeSupport and check minDFS
</commit_message>
<xml_diff>
--- a/MyThesis.xlsx
+++ b/MyThesis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6870" firstSheet="13" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6870" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -150,6 +150,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Bencat</author>
+    <author>BinhTruong</author>
   </authors>
   <commentList>
     <comment ref="B25" authorId="0" shapeId="0">
@@ -286,6 +287,30 @@
           </rPr>
           <t xml:space="preserve">
 =(i%(Le*Lv)-(((i%(Le*Lv))/Lv)*Lv)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B53" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>BinhTruong:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+=INT(i/Lv)</t>
         </r>
       </text>
     </comment>
@@ -1594,7 +1619,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="496">
   <si>
     <t>A</t>
   </si>
@@ -3451,6 +3476,9 @@
   </si>
   <si>
     <t>toIndex_V:--&gt;</t>
+  </si>
+  <si>
+    <t>Chỉ xét 1 tập đỉnh:</t>
   </si>
 </sst>
 </file>
@@ -5080,6 +5108,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5215,30 +5267,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13092,7 +13120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
@@ -13218,11 +13246,11 @@
       <c r="H19" s="91">
         <v>0</v>
       </c>
-      <c r="J19" s="285" t="s">
+      <c r="J19" s="297" t="s">
         <v>301</v>
       </c>
-      <c r="K19" s="286"/>
-      <c r="L19" s="287"/>
+      <c r="K19" s="298"/>
+      <c r="L19" s="299"/>
       <c r="N19" s="173" t="s">
         <v>315</v>
       </c>
@@ -13389,7 +13417,7 @@
       <c r="L34" s="176" t="s">
         <v>322</v>
       </c>
-      <c r="M34" s="288" t="s">
+      <c r="M34" s="300" t="s">
         <v>325</v>
       </c>
       <c r="N34" s="175" t="s">
@@ -13409,7 +13437,7 @@
       <c r="L35" s="176" t="s">
         <v>326</v>
       </c>
-      <c r="M35" s="288"/>
+      <c r="M35" s="300"/>
       <c r="N35" s="175" t="s">
         <v>117</v>
       </c>
@@ -13959,14 +13987,14 @@
       <c r="A10" s="156"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="289" t="s">
+      <c r="B11" s="301" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="290"/>
-      <c r="E11" s="289" t="s">
+      <c r="C11" s="302"/>
+      <c r="E11" s="301" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="290"/>
+      <c r="F11" s="302"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="165" t="s">
@@ -14295,8 +14323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:S187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53:M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14511,26 +14539,26 @@
       <c r="A27" s="137" t="s">
         <v>380</v>
       </c>
-      <c r="B27" s="310">
-        <v>0</v>
-      </c>
-      <c r="C27" s="311"/>
-      <c r="D27" s="312"/>
-      <c r="E27" s="310">
-        <v>0</v>
-      </c>
-      <c r="F27" s="311"/>
-      <c r="G27" s="312"/>
-      <c r="H27" s="310">
+      <c r="B27" s="322">
+        <v>0</v>
+      </c>
+      <c r="C27" s="323"/>
+      <c r="D27" s="324"/>
+      <c r="E27" s="322">
+        <v>0</v>
+      </c>
+      <c r="F27" s="323"/>
+      <c r="G27" s="324"/>
+      <c r="H27" s="322">
         <v>5</v>
       </c>
-      <c r="I27" s="311"/>
-      <c r="J27" s="312"/>
-      <c r="K27" s="305">
+      <c r="I27" s="323"/>
+      <c r="J27" s="324"/>
+      <c r="K27" s="317">
         <v>13</v>
       </c>
-      <c r="L27" s="311"/>
-      <c r="M27" s="312"/>
+      <c r="L27" s="323"/>
+      <c r="M27" s="324"/>
       <c r="N27" s="159" t="s">
         <v>491</v>
       </c>
@@ -14554,26 +14582,26 @@
       <c r="A28" s="137" t="s">
         <v>381</v>
       </c>
-      <c r="B28" s="313" t="s">
+      <c r="B28" s="325" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="297"/>
-      <c r="D28" s="314"/>
-      <c r="E28" s="315" t="s">
+      <c r="C28" s="309"/>
+      <c r="D28" s="326"/>
+      <c r="E28" s="327" t="s">
         <v>73</v>
       </c>
-      <c r="F28" s="316"/>
-      <c r="G28" s="317"/>
-      <c r="H28" s="315" t="s">
+      <c r="F28" s="328"/>
+      <c r="G28" s="329"/>
+      <c r="H28" s="327" t="s">
         <v>79</v>
       </c>
-      <c r="I28" s="316"/>
-      <c r="J28" s="317"/>
-      <c r="K28" s="318" t="s">
+      <c r="I28" s="328"/>
+      <c r="J28" s="329"/>
+      <c r="K28" s="330" t="s">
         <v>90</v>
       </c>
-      <c r="L28" s="316"/>
-      <c r="M28" s="317"/>
+      <c r="L28" s="328"/>
+      <c r="M28" s="329"/>
       <c r="N28" s="159" t="s">
         <v>493</v>
       </c>
@@ -14643,7 +14671,7 @@
         <v>2</v>
       </c>
       <c r="P29" s="1">
-        <f t="shared" ref="P29:Q29" si="1">Q27*$O$26-1</f>
+        <f t="shared" ref="P29" si="1">Q27*$O$26-1</f>
         <v>5</v>
       </c>
       <c r="Q29" s="1">
@@ -14942,21 +14970,21 @@
       <c r="A42" t="s">
         <v>403</v>
       </c>
-      <c r="B42" s="283" t="s">
+      <c r="B42" s="295" t="s">
         <v>125</v>
       </c>
-      <c r="C42" s="278"/>
-      <c r="D42" s="309"/>
-      <c r="E42" s="283" t="s">
+      <c r="C42" s="290"/>
+      <c r="D42" s="321"/>
+      <c r="E42" s="295" t="s">
         <v>126</v>
       </c>
-      <c r="F42" s="278"/>
-      <c r="G42" s="279"/>
-      <c r="H42" s="277" t="s">
+      <c r="F42" s="290"/>
+      <c r="G42" s="291"/>
+      <c r="H42" s="289" t="s">
         <v>127</v>
       </c>
-      <c r="I42" s="278"/>
-      <c r="J42" s="279"/>
+      <c r="I42" s="290"/>
+      <c r="J42" s="291"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -15023,24 +15051,24 @@
       <c r="A45" t="s">
         <v>404</v>
       </c>
-      <c r="B45" s="293">
+      <c r="B45" s="305">
         <f>SUM(B43:D43)</f>
         <v>1</v>
       </c>
-      <c r="C45" s="306"/>
-      <c r="D45" s="307"/>
-      <c r="E45" s="293">
+      <c r="C45" s="318"/>
+      <c r="D45" s="319"/>
+      <c r="E45" s="305">
         <f t="shared" ref="E45" si="4">SUM(E43:G43)</f>
         <v>1</v>
       </c>
-      <c r="F45" s="306"/>
-      <c r="G45" s="294"/>
-      <c r="H45" s="308">
+      <c r="F45" s="318"/>
+      <c r="G45" s="306"/>
+      <c r="H45" s="320">
         <f t="shared" ref="H45" si="5">SUM(H43:J43)</f>
         <v>1</v>
       </c>
-      <c r="I45" s="306"/>
-      <c r="J45" s="294"/>
+      <c r="I45" s="318"/>
+      <c r="J45" s="306"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="208">
@@ -15125,51 +15153,51 @@
       <c r="A49" s="137" t="s">
         <v>396</v>
       </c>
-      <c r="B49" s="310">
-        <v>1</v>
-      </c>
-      <c r="C49" s="311"/>
-      <c r="D49" s="312"/>
-      <c r="E49" s="305">
-        <v>2</v>
-      </c>
-      <c r="F49" s="311"/>
-      <c r="G49" s="304"/>
-      <c r="H49" s="310">
+      <c r="B49" s="322">
+        <v>1</v>
+      </c>
+      <c r="C49" s="323"/>
+      <c r="D49" s="324"/>
+      <c r="E49" s="317">
+        <v>2</v>
+      </c>
+      <c r="F49" s="323"/>
+      <c r="G49" s="316"/>
+      <c r="H49" s="322">
         <v>6</v>
       </c>
-      <c r="I49" s="311"/>
-      <c r="J49" s="312"/>
-      <c r="K49" s="305">
+      <c r="I49" s="323"/>
+      <c r="J49" s="324"/>
+      <c r="K49" s="317">
         <v>10</v>
       </c>
-      <c r="L49" s="311"/>
-      <c r="M49" s="312"/>
+      <c r="L49" s="323"/>
+      <c r="M49" s="324"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="137" t="s">
         <v>381</v>
       </c>
-      <c r="B50" s="313" t="s">
+      <c r="B50" s="325" t="s">
         <v>71</v>
       </c>
-      <c r="C50" s="297"/>
-      <c r="D50" s="314"/>
-      <c r="E50" s="318" t="s">
+      <c r="C50" s="309"/>
+      <c r="D50" s="326"/>
+      <c r="E50" s="330" t="s">
         <v>73</v>
       </c>
-      <c r="F50" s="316"/>
-      <c r="G50" s="319"/>
-      <c r="H50" s="315" t="s">
+      <c r="F50" s="328"/>
+      <c r="G50" s="331"/>
+      <c r="H50" s="327" t="s">
         <v>79</v>
       </c>
-      <c r="I50" s="316"/>
-      <c r="J50" s="317"/>
-      <c r="K50" s="318" t="s">
+      <c r="I50" s="328"/>
+      <c r="J50" s="329"/>
+      <c r="K50" s="330" t="s">
         <v>90</v>
       </c>
-      <c r="L50" s="316"/>
-      <c r="M50" s="317"/>
+      <c r="L50" s="328"/>
+      <c r="M50" s="329"/>
     </row>
     <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="137" t="s">
@@ -15619,10 +15647,10 @@
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B64" s="291" t="s">
+      <c r="B64" s="303" t="s">
         <v>411</v>
       </c>
-      <c r="C64" s="292"/>
+      <c r="C64" s="304"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B65" s="246" t="s">
@@ -15735,21 +15763,21 @@
       <c r="A75" t="s">
         <v>403</v>
       </c>
-      <c r="B75" s="283" t="s">
+      <c r="B75" s="295" t="s">
         <v>130</v>
       </c>
-      <c r="C75" s="278"/>
-      <c r="D75" s="309"/>
-      <c r="E75" s="283" t="s">
+      <c r="C75" s="290"/>
+      <c r="D75" s="321"/>
+      <c r="E75" s="295" t="s">
         <v>131</v>
       </c>
-      <c r="F75" s="278"/>
-      <c r="G75" s="279"/>
-      <c r="H75" s="277" t="s">
+      <c r="F75" s="290"/>
+      <c r="G75" s="291"/>
+      <c r="H75" s="289" t="s">
         <v>132</v>
       </c>
-      <c r="I75" s="278"/>
-      <c r="J75" s="279"/>
+      <c r="I75" s="290"/>
+      <c r="J75" s="291"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
@@ -15816,24 +15844,24 @@
       <c r="A78" t="s">
         <v>404</v>
       </c>
-      <c r="B78" s="293">
+      <c r="B78" s="305">
         <f>SUM(B76:D76)</f>
         <v>1</v>
       </c>
-      <c r="C78" s="306"/>
-      <c r="D78" s="307"/>
-      <c r="E78" s="293">
+      <c r="C78" s="318"/>
+      <c r="D78" s="319"/>
+      <c r="E78" s="305">
         <f t="shared" ref="E78" si="10">SUM(E76:G76)</f>
         <v>1</v>
       </c>
-      <c r="F78" s="306"/>
-      <c r="G78" s="294"/>
-      <c r="H78" s="308">
+      <c r="F78" s="318"/>
+      <c r="G78" s="306"/>
+      <c r="H78" s="320">
         <f t="shared" ref="H78" si="11">SUM(H76:J76)</f>
         <v>2</v>
       </c>
-      <c r="I78" s="306"/>
-      <c r="J78" s="294"/>
+      <c r="I78" s="318"/>
+      <c r="J78" s="306"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H80" t="s">
@@ -16010,59 +16038,59 @@
       <c r="A92" s="137" t="s">
         <v>414</v>
       </c>
-      <c r="B92" s="304">
+      <c r="B92" s="316">
         <v>3</v>
       </c>
-      <c r="C92" s="305"/>
-      <c r="D92" s="304">
-        <v>4</v>
-      </c>
-      <c r="E92" s="305"/>
-      <c r="F92" s="304">
+      <c r="C92" s="317"/>
+      <c r="D92" s="316">
+        <v>4</v>
+      </c>
+      <c r="E92" s="317"/>
+      <c r="F92" s="316">
         <v>3</v>
       </c>
-      <c r="G92" s="305"/>
-      <c r="H92" s="304">
-        <v>4</v>
-      </c>
-      <c r="I92" s="305"/>
-      <c r="J92" s="304">
+      <c r="G92" s="317"/>
+      <c r="H92" s="316">
+        <v>4</v>
+      </c>
+      <c r="I92" s="317"/>
+      <c r="J92" s="316">
         <v>11</v>
       </c>
-      <c r="K92" s="305"/>
-      <c r="L92" s="304">
+      <c r="K92" s="317"/>
+      <c r="L92" s="316">
         <v>12</v>
       </c>
-      <c r="M92" s="305"/>
+      <c r="M92" s="317"/>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="137" t="s">
         <v>381</v>
       </c>
-      <c r="B93" s="298" t="s">
+      <c r="B93" s="310" t="s">
         <v>415</v>
       </c>
-      <c r="C93" s="296"/>
-      <c r="D93" s="298" t="s">
+      <c r="C93" s="308"/>
+      <c r="D93" s="310" t="s">
         <v>416</v>
       </c>
-      <c r="E93" s="296"/>
-      <c r="F93" s="298" t="s">
+      <c r="E93" s="308"/>
+      <c r="F93" s="310" t="s">
         <v>417</v>
       </c>
-      <c r="G93" s="296"/>
-      <c r="H93" s="298" t="s">
+      <c r="G93" s="308"/>
+      <c r="H93" s="310" t="s">
         <v>418</v>
       </c>
-      <c r="I93" s="296"/>
-      <c r="J93" s="298" t="s">
+      <c r="I93" s="308"/>
+      <c r="J93" s="310" t="s">
         <v>419</v>
       </c>
-      <c r="K93" s="296"/>
-      <c r="L93" s="298" t="s">
+      <c r="K93" s="308"/>
+      <c r="L93" s="310" t="s">
         <v>420</v>
       </c>
-      <c r="M93" s="296"/>
+      <c r="M93" s="308"/>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="137" t="s">
@@ -16463,10 +16491,10 @@
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B109" s="291" t="s">
+      <c r="B109" s="303" t="s">
         <v>433</v>
       </c>
-      <c r="C109" s="292"/>
+      <c r="C109" s="304"/>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B110" s="246" t="s">
@@ -16536,14 +16564,14 @@
       <c r="A120" t="s">
         <v>403</v>
       </c>
-      <c r="B120" s="299" t="s">
+      <c r="B120" s="311" t="s">
         <v>423</v>
       </c>
-      <c r="C120" s="300"/>
-      <c r="D120" s="301" t="s">
+      <c r="C120" s="312"/>
+      <c r="D120" s="313" t="s">
         <v>421</v>
       </c>
-      <c r="E120" s="300"/>
+      <c r="E120" s="312"/>
       <c r="F120" s="254"/>
       <c r="G120" s="254"/>
       <c r="H120" s="254"/>
@@ -16598,16 +16626,16 @@
       <c r="A123" t="s">
         <v>404</v>
       </c>
-      <c r="B123" s="302">
+      <c r="B123" s="314">
         <f>SUM(B121:C121)</f>
         <v>1</v>
       </c>
-      <c r="C123" s="303"/>
-      <c r="D123" s="302">
+      <c r="C123" s="315"/>
+      <c r="D123" s="314">
         <f>SUM(D121:E121)</f>
         <v>1</v>
       </c>
-      <c r="E123" s="303"/>
+      <c r="E123" s="315"/>
       <c r="F123" s="256"/>
       <c r="G123" s="256"/>
       <c r="H123" s="256"/>
@@ -16733,71 +16761,71 @@
       <c r="A128" s="137" t="s">
         <v>396</v>
       </c>
-      <c r="B128" s="298">
-        <v>1</v>
-      </c>
-      <c r="C128" s="295"/>
-      <c r="D128" s="296"/>
-      <c r="E128" s="298">
-        <v>1</v>
-      </c>
-      <c r="F128" s="295"/>
-      <c r="G128" s="296"/>
-      <c r="H128" s="297">
-        <v>2</v>
-      </c>
-      <c r="I128" s="297"/>
-      <c r="J128" s="297"/>
-      <c r="K128" s="297">
-        <v>2</v>
-      </c>
-      <c r="L128" s="297"/>
-      <c r="M128" s="297"/>
-      <c r="N128" s="297">
+      <c r="B128" s="310">
+        <v>1</v>
+      </c>
+      <c r="C128" s="307"/>
+      <c r="D128" s="308"/>
+      <c r="E128" s="310">
+        <v>1</v>
+      </c>
+      <c r="F128" s="307"/>
+      <c r="G128" s="308"/>
+      <c r="H128" s="309">
+        <v>2</v>
+      </c>
+      <c r="I128" s="309"/>
+      <c r="J128" s="309"/>
+      <c r="K128" s="309">
+        <v>2</v>
+      </c>
+      <c r="L128" s="309"/>
+      <c r="M128" s="309"/>
+      <c r="N128" s="309">
         <v>10</v>
       </c>
-      <c r="O128" s="297"/>
-      <c r="P128" s="297"/>
-      <c r="Q128" s="295">
+      <c r="O128" s="309"/>
+      <c r="P128" s="309"/>
+      <c r="Q128" s="307">
         <v>10</v>
       </c>
-      <c r="R128" s="295"/>
-      <c r="S128" s="296"/>
+      <c r="R128" s="307"/>
+      <c r="S128" s="308"/>
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" s="137" t="s">
         <v>381</v>
       </c>
-      <c r="B129" s="298" t="s">
+      <c r="B129" s="310" t="s">
         <v>415</v>
       </c>
-      <c r="C129" s="295"/>
-      <c r="D129" s="296"/>
-      <c r="E129" s="298" t="s">
+      <c r="C129" s="307"/>
+      <c r="D129" s="308"/>
+      <c r="E129" s="310" t="s">
         <v>416</v>
       </c>
-      <c r="F129" s="295"/>
-      <c r="G129" s="296"/>
-      <c r="H129" s="297" t="s">
+      <c r="F129" s="307"/>
+      <c r="G129" s="308"/>
+      <c r="H129" s="309" t="s">
         <v>417</v>
       </c>
-      <c r="I129" s="297"/>
-      <c r="J129" s="297"/>
-      <c r="K129" s="297" t="s">
+      <c r="I129" s="309"/>
+      <c r="J129" s="309"/>
+      <c r="K129" s="309" t="s">
         <v>418</v>
       </c>
-      <c r="L129" s="297"/>
-      <c r="M129" s="297"/>
-      <c r="N129" s="297" t="s">
+      <c r="L129" s="309"/>
+      <c r="M129" s="309"/>
+      <c r="N129" s="309" t="s">
         <v>419</v>
       </c>
-      <c r="O129" s="297"/>
-      <c r="P129" s="297"/>
-      <c r="Q129" s="295" t="s">
+      <c r="O129" s="309"/>
+      <c r="P129" s="309"/>
+      <c r="Q129" s="307" t="s">
         <v>420</v>
       </c>
-      <c r="R129" s="295"/>
-      <c r="S129" s="296"/>
+      <c r="R129" s="307"/>
+      <c r="S129" s="308"/>
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" s="137" t="s">
@@ -17213,10 +17241,10 @@
     </row>
     <row r="144" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B145" s="291" t="s">
+      <c r="B145" s="303" t="s">
         <v>433</v>
       </c>
-      <c r="C145" s="292"/>
+      <c r="C145" s="304"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B146" s="246" t="s">
@@ -17302,10 +17330,10 @@
       <c r="A156" t="s">
         <v>403</v>
       </c>
-      <c r="B156" s="283" t="s">
+      <c r="B156" s="295" t="s">
         <v>132</v>
       </c>
-      <c r="C156" s="279"/>
+      <c r="C156" s="291"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
@@ -17333,11 +17361,11 @@
       <c r="A159" t="s">
         <v>404</v>
       </c>
-      <c r="B159" s="293">
+      <c r="B159" s="305">
         <f>SUM(B157:C157)</f>
         <v>2</v>
       </c>
-      <c r="C159" s="294"/>
+      <c r="C159" s="306"/>
     </row>
     <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B162" s="235">
@@ -17458,71 +17486,71 @@
       <c r="A164" s="137" t="s">
         <v>380</v>
       </c>
-      <c r="B164" s="298">
-        <v>0</v>
-      </c>
-      <c r="C164" s="295"/>
-      <c r="D164" s="296"/>
-      <c r="E164" s="298">
-        <v>0</v>
-      </c>
-      <c r="F164" s="295"/>
-      <c r="G164" s="296"/>
-      <c r="H164" s="297">
-        <v>0</v>
-      </c>
-      <c r="I164" s="297"/>
-      <c r="J164" s="297"/>
-      <c r="K164" s="297">
-        <v>0</v>
-      </c>
-      <c r="L164" s="297"/>
-      <c r="M164" s="297"/>
-      <c r="N164" s="297">
+      <c r="B164" s="310">
+        <v>0</v>
+      </c>
+      <c r="C164" s="307"/>
+      <c r="D164" s="308"/>
+      <c r="E164" s="310">
+        <v>0</v>
+      </c>
+      <c r="F164" s="307"/>
+      <c r="G164" s="308"/>
+      <c r="H164" s="309">
+        <v>0</v>
+      </c>
+      <c r="I164" s="309"/>
+      <c r="J164" s="309"/>
+      <c r="K164" s="309">
+        <v>0</v>
+      </c>
+      <c r="L164" s="309"/>
+      <c r="M164" s="309"/>
+      <c r="N164" s="309">
         <v>13</v>
       </c>
-      <c r="O164" s="297"/>
-      <c r="P164" s="297"/>
-      <c r="Q164" s="295">
+      <c r="O164" s="309"/>
+      <c r="P164" s="309"/>
+      <c r="Q164" s="307">
         <v>13</v>
       </c>
-      <c r="R164" s="295"/>
-      <c r="S164" s="296"/>
+      <c r="R164" s="307"/>
+      <c r="S164" s="308"/>
     </row>
     <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165" s="137" t="s">
         <v>381</v>
       </c>
-      <c r="B165" s="298" t="s">
+      <c r="B165" s="310" t="s">
         <v>415</v>
       </c>
-      <c r="C165" s="295"/>
-      <c r="D165" s="296"/>
-      <c r="E165" s="298" t="s">
+      <c r="C165" s="307"/>
+      <c r="D165" s="308"/>
+      <c r="E165" s="310" t="s">
         <v>416</v>
       </c>
-      <c r="F165" s="295"/>
-      <c r="G165" s="296"/>
-      <c r="H165" s="297" t="s">
+      <c r="F165" s="307"/>
+      <c r="G165" s="308"/>
+      <c r="H165" s="309" t="s">
         <v>417</v>
       </c>
-      <c r="I165" s="297"/>
-      <c r="J165" s="297"/>
-      <c r="K165" s="297" t="s">
+      <c r="I165" s="309"/>
+      <c r="J165" s="309"/>
+      <c r="K165" s="309" t="s">
         <v>418</v>
       </c>
-      <c r="L165" s="297"/>
-      <c r="M165" s="297"/>
-      <c r="N165" s="297" t="s">
+      <c r="L165" s="309"/>
+      <c r="M165" s="309"/>
+      <c r="N165" s="309" t="s">
         <v>419</v>
       </c>
-      <c r="O165" s="297"/>
-      <c r="P165" s="297"/>
-      <c r="Q165" s="295" t="s">
+      <c r="O165" s="309"/>
+      <c r="P165" s="309"/>
+      <c r="Q165" s="307" t="s">
         <v>420</v>
       </c>
-      <c r="R165" s="295"/>
-      <c r="S165" s="296"/>
+      <c r="R165" s="307"/>
+      <c r="S165" s="308"/>
     </row>
     <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" s="137" t="s">
@@ -18242,7 +18270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Z25"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
@@ -18697,7 +18725,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18713,59 +18741,59 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="324" t="s">
+      <c r="B2" s="279" t="s">
         <v>465</v>
       </c>
-      <c r="C2" s="324" t="s">
+      <c r="C2" s="279" t="s">
         <v>466</v>
       </c>
-      <c r="D2" s="324" t="s">
+      <c r="D2" s="279" t="s">
         <v>467</v>
       </c>
-      <c r="E2" s="324" t="s">
+      <c r="E2" s="279" t="s">
         <v>468</v>
       </c>
-      <c r="F2" s="324" t="s">
+      <c r="F2" s="279" t="s">
         <v>469</v>
       </c>
-      <c r="G2" s="324" t="s">
+      <c r="G2" s="279" t="s">
         <v>470</v>
       </c>
-      <c r="H2" s="324" t="s">
+      <c r="H2" s="279" t="s">
         <v>471</v>
       </c>
-      <c r="I2" s="320" t="s">
+      <c r="I2" s="275" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="322" t="s">
+      <c r="B3" s="277" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="325" t="s">
+      <c r="C3" s="280" t="s">
         <v>473</v>
       </c>
-      <c r="D3" s="325" t="s">
+      <c r="D3" s="280" t="s">
         <v>474</v>
       </c>
-      <c r="E3" s="325" t="s">
+      <c r="E3" s="280" t="s">
         <v>475</v>
       </c>
-      <c r="F3" s="325" t="s">
+      <c r="F3" s="280" t="s">
         <v>476</v>
       </c>
-      <c r="G3" s="325" t="s">
+      <c r="G3" s="280" t="s">
         <v>477</v>
       </c>
-      <c r="H3" s="325" t="s">
+      <c r="H3" s="280" t="s">
         <v>478</v>
       </c>
-      <c r="I3" s="320" t="s">
+      <c r="I3" s="275" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="322" t="s">
+      <c r="B4" s="277" t="s">
         <v>102</v>
       </c>
       <c r="C4" s="274">
@@ -18786,15 +18814,15 @@
       <c r="H4" s="274">
         <v>11</v>
       </c>
-      <c r="I4" s="321" t="s">
+      <c r="I4" s="276" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="323" t="s">
+      <c r="A5" s="278" t="s">
         <v>375</v>
       </c>
-      <c r="B5" s="322" t="s">
+      <c r="B5" s="277" t="s">
         <v>463</v>
       </c>
       <c r="C5" s="274">
@@ -18815,7 +18843,7 @@
       <c r="H5" s="274">
         <v>17</v>
       </c>
-      <c r="I5" s="321" t="s">
+      <c r="I5" s="276" t="s">
         <v>463</v>
       </c>
     </row>
@@ -18841,11 +18869,11 @@
       <c r="C11" t="s">
         <v>483</v>
       </c>
-      <c r="F11" s="327"/>
+      <c r="F11" s="282"/>
       <c r="I11" t="s">
         <v>484</v>
       </c>
-      <c r="L11" s="327"/>
+      <c r="L11" s="282"/>
       <c r="O11" t="s">
         <v>485</v>
       </c>
@@ -19028,25 +19056,25 @@
       <c r="L15" s="273">
         <v>3</v>
       </c>
-      <c r="M15" s="328">
-        <v>0</v>
-      </c>
-      <c r="N15" s="328">
-        <v>0</v>
-      </c>
-      <c r="O15" s="328">
-        <v>1</v>
-      </c>
-      <c r="P15" s="328">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="328">
+      <c r="M15" s="283">
+        <v>0</v>
+      </c>
+      <c r="N15" s="283">
+        <v>0</v>
+      </c>
+      <c r="O15" s="283">
+        <v>1</v>
+      </c>
+      <c r="P15" s="283">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="283">
         <v>3</v>
       </c>
-      <c r="R15" s="328">
+      <c r="R15" s="283">
         <v>3</v>
       </c>
-      <c r="S15" s="329" t="s">
+      <c r="S15" s="284" t="s">
         <v>488</v>
       </c>
     </row>
@@ -19123,7 +19151,7 @@
         <f t="shared" si="3"/>
         <v>Q0[3]</v>
       </c>
-      <c r="S16" s="326" t="s">
+      <c r="S16" s="281" t="s">
         <v>489</v>
       </c>
     </row>
@@ -19170,27 +19198,27 @@
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="M17" s="328">
+      <c r="M17" s="283">
         <f>MOD(M12,6)</f>
         <v>0</v>
       </c>
-      <c r="N17" s="328">
+      <c r="N17" s="283">
         <f t="shared" ref="N17:R17" si="5">MOD(N12,6)</f>
         <v>1</v>
       </c>
-      <c r="O17" s="328">
+      <c r="O17" s="283">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="P17" s="328">
+      <c r="P17" s="283">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="Q17" s="328">
+      <c r="Q17" s="283">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="R17" s="328">
+      <c r="R17" s="283">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
@@ -19511,36 +19539,36 @@
       <c r="B35" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="283" t="s">
+      <c r="C35" s="295" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="278"/>
-      <c r="E35" s="279"/>
-      <c r="F35" s="283" t="s">
+      <c r="D35" s="290"/>
+      <c r="E35" s="291"/>
+      <c r="F35" s="295" t="s">
         <v>74</v>
       </c>
-      <c r="G35" s="278"/>
-      <c r="H35" s="279"/>
-      <c r="I35" s="283" t="s">
+      <c r="G35" s="290"/>
+      <c r="H35" s="291"/>
+      <c r="I35" s="295" t="s">
         <v>80</v>
       </c>
-      <c r="J35" s="278"/>
-      <c r="K35" s="279"/>
-      <c r="L35" s="283" t="s">
+      <c r="J35" s="290"/>
+      <c r="K35" s="291"/>
+      <c r="L35" s="295" t="s">
         <v>82</v>
       </c>
-      <c r="M35" s="278"/>
-      <c r="N35" s="279"/>
-      <c r="O35" s="283" t="s">
+      <c r="M35" s="290"/>
+      <c r="N35" s="291"/>
+      <c r="O35" s="295" t="s">
         <v>84</v>
       </c>
-      <c r="P35" s="278"/>
-      <c r="Q35" s="279"/>
-      <c r="R35" s="277" t="s">
+      <c r="P35" s="290"/>
+      <c r="Q35" s="291"/>
+      <c r="R35" s="289" t="s">
         <v>91</v>
       </c>
-      <c r="S35" s="278"/>
-      <c r="T35" s="279"/>
+      <c r="S35" s="290"/>
+      <c r="T35" s="291"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B36" s="50" t="s">
@@ -19683,16 +19711,16 @@
       <c r="B48" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="280" t="s">
+      <c r="C48" s="292" t="s">
         <v>70</v>
       </c>
-      <c r="D48" s="281"/>
-      <c r="E48" s="282"/>
-      <c r="F48" s="283" t="s">
+      <c r="D48" s="293"/>
+      <c r="E48" s="294"/>
+      <c r="F48" s="295" t="s">
         <v>74</v>
       </c>
-      <c r="G48" s="278"/>
-      <c r="H48" s="279"/>
+      <c r="G48" s="290"/>
+      <c r="H48" s="291"/>
     </row>
     <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" s="33" t="s">
@@ -20057,14 +20085,14 @@
     </row>
     <row r="58" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="275" t="s">
+      <c r="C59" s="287" t="s">
         <v>102</v>
       </c>
-      <c r="D59" s="276"/>
-      <c r="F59" s="275" t="s">
+      <c r="D59" s="288"/>
+      <c r="F59" s="287" t="s">
         <v>103</v>
       </c>
-      <c r="G59" s="276"/>
+      <c r="G59" s="288"/>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B60">
@@ -23115,28 +23143,28 @@
       <c r="E7" s="111">
         <v>1</v>
       </c>
-      <c r="F7" s="330">
+      <c r="F7" s="285">
         <f>E9+F9</f>
         <v>2</v>
       </c>
       <c r="G7" s="111">
         <v>0</v>
       </c>
-      <c r="H7" s="330">
+      <c r="H7" s="285">
         <f>G9+H9</f>
         <v>0</v>
       </c>
       <c r="I7" s="111">
         <v>1</v>
       </c>
-      <c r="J7" s="330">
+      <c r="J7" s="285">
         <f>I9+J9</f>
         <v>2</v>
       </c>
       <c r="K7" s="111">
         <v>0</v>
       </c>
-      <c r="L7" s="331">
+      <c r="L7" s="286">
         <f>K9+L9</f>
         <v>1</v>
       </c>
@@ -24702,7 +24730,7 @@
         <v>2</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="D7:AG7" si="4">E7+E3</f>
+        <f t="shared" ref="F7:AG7" si="4">E7+E3</f>
         <v>2</v>
       </c>
       <c r="G7">
@@ -24832,7 +24860,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="131">
-        <f t="shared" ref="C9:H9" si="5">D4</f>
+        <f t="shared" ref="D9:H9" si="5">D4</f>
         <v>2</v>
       </c>
       <c r="E9" s="131">
@@ -25214,16 +25242,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ52"/>
+  <dimension ref="A1:AZ54"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="AC16" sqref="AC16"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54:L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="159" bestFit="1" customWidth="1"/>
-    <col min="2" max="33" width="4.7109375" customWidth="1"/>
+    <col min="2" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="33" width="4.7109375" customWidth="1"/>
     <col min="34" max="34" width="5.5703125" customWidth="1"/>
     <col min="35" max="42" width="4.85546875" customWidth="1"/>
     <col min="43" max="52" width="3.85546875" customWidth="1"/>
@@ -28818,10 +28848,10 @@
       </c>
     </row>
     <row r="49" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A49" s="284" t="s">
+      <c r="A49" s="296" t="s">
         <v>271</v>
       </c>
-      <c r="B49" s="284"/>
+      <c r="B49" s="296"/>
       <c r="C49">
         <f>C48/5</f>
         <v>0</v>
@@ -29436,6 +29466,99 @@
     <row r="52" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>272</v>
+      </c>
+    </row>
+    <row r="53" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A53" s="159" t="s">
+        <v>495</v>
+      </c>
+      <c r="B53" t="s">
+        <v>263</v>
+      </c>
+      <c r="C53">
+        <f>INT(C48/($F$36))</f>
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <f t="shared" ref="D53:L53" si="105">INT(D48/($F$36))</f>
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="105"/>
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="105"/>
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="105"/>
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="105"/>
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="105"/>
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="105"/>
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="105"/>
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="105"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>257</v>
+      </c>
+      <c r="C54">
+        <f>MOD(C48,$F$36)</f>
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <f t="shared" ref="D54:L54" si="106">MOD(D48,$F$36)</f>
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="106"/>
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="106"/>
+        <v>3</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="106"/>
+        <v>4</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="106"/>
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="106"/>
+        <v>2</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="106"/>
+        <v>3</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="106"/>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>